<commit_message>
loops over all policies
</commit_message>
<xml_diff>
--- a/param_files/Epi_parameters_June_24_2020.xlsx
+++ b/param_files/Epi_parameters_June_24_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/GitHub/epi_model_HIV_TB/param_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D7A442-DBCC-AD40-95A4-EFAF2B0DBBC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5849E5-6A8C-1648-9ECA-60CF49D11E0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Matched_Parameters" sheetId="1" r:id="rId1"/>
@@ -1386,22 +1386,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O194"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="10" ySplit="1" topLeftCell="K27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="69.33203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="53" style="9" customWidth="1"/>
-    <col min="3" max="4" width="7.83203125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="14" style="9" customWidth="1"/>
-    <col min="6" max="7" width="15" style="9" customWidth="1"/>
-    <col min="8" max="8" width="26" style="9" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="53" style="9" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="7.83203125" style="9" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="9" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="15" style="9" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="26" style="9" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="9" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="22.33203125" style="9" customWidth="1"/>
     <col min="11" max="11" width="20" style="9" customWidth="1"/>
     <col min="12" max="12" width="17.83203125" style="9" customWidth="1"/>
@@ -7603,20 +7603,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C936F566-E80E-414B-9865-88FE42A54FD2}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
-    </sheetView>
+    <sheetView topLeftCell="A20" zoomScale="151" zoomScaleNormal="151" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="52.1640625" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="14" style="9" customWidth="1"/>
-    <col min="4" max="5" width="15" style="9" customWidth="1"/>
-    <col min="6" max="6" width="26" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="9" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="9" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="15" style="9" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="26" style="9" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="22.33203125" style="9" customWidth="1"/>
     <col min="8" max="9" width="17.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.83203125" style="1" customWidth="1"/>
@@ -7661,7 +7658,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32" hidden="1">
+    <row r="2" spans="1:12" ht="32">
       <c r="A2" s="1" t="str">
         <f t="shared" ref="A2:A33" si="0">CONCATENATE("Population in TB compartment ",VLOOKUP(C2,TB_SET,2), " with ", VLOOKUP(D2,R_SET,2), " in HIV compartment ", VLOOKUP(E2,HIV_SET,2), " and ", VLOOKUP(F2, G_SET,2))</f>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -7694,7 +7691,7 @@
         <v>2946.4285714285788</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="48" hidden="1">
+    <row r="3" spans="1:12" ht="48">
       <c r="A3" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -7726,7 +7723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="32" hidden="1">
+    <row r="4" spans="1:12" ht="32">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -7759,7 +7756,7 @@
         <v>2946.4285714285788</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="48" hidden="1">
+    <row r="5" spans="1:12" ht="48">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -7791,7 +7788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="48" hidden="1">
+    <row r="6" spans="1:12" ht="48">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -7857,7 +7854,7 @@
         <v>2946.4285714285788</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="32" hidden="1">
+    <row r="8" spans="1:12" ht="32">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -7890,7 +7887,7 @@
         <v>2946.4285714285788</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="48" hidden="1">
+    <row r="9" spans="1:12" ht="48">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -7923,7 +7920,7 @@
         <v>2946.4285714285788</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="32" hidden="1">
+    <row r="10" spans="1:12" ht="32">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -7956,7 +7953,7 @@
         <v>2946.4285714285788</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="32" hidden="1">
+    <row r="11" spans="1:12" ht="32">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -7989,7 +7986,7 @@
         <v>2946.4285714285788</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="32" hidden="1">
+    <row r="12" spans="1:12" ht="32">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8022,7 +8019,7 @@
         <v>2946.4285714285788</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="32" hidden="1">
+    <row r="13" spans="1:12" ht="32">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8055,7 +8052,7 @@
         <v>2946.4285714285788</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="32" hidden="1">
+    <row r="14" spans="1:12" ht="32">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8088,7 +8085,7 @@
         <v>2946.4285714285788</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="48" hidden="1">
+    <row r="15" spans="1:12" ht="48">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8121,7 +8118,7 @@
         <v>2946.4285714285788</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="32" hidden="1">
+    <row r="16" spans="1:12" ht="32">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8154,7 +8151,7 @@
         <v>2946.4285714285788</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="32" hidden="1">
+    <row r="17" spans="1:9" ht="32">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8187,7 +8184,7 @@
         <v>2946.4285714285788</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="48" hidden="1">
+    <row r="18" spans="1:9" ht="48">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8220,7 +8217,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="48" hidden="1">
+    <row r="19" spans="1:9" ht="48">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -8252,7 +8249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="48" hidden="1">
+    <row r="20" spans="1:9" ht="48">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8285,7 +8282,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="48" hidden="1">
+    <row r="21" spans="1:9" ht="48">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -8317,7 +8314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="48" hidden="1">
+    <row r="22" spans="1:9" ht="48">
       <c r="A22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8383,7 +8380,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="48" hidden="1">
+    <row r="24" spans="1:9" ht="48">
       <c r="A24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8416,7 +8413,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="48" hidden="1">
+    <row r="25" spans="1:9" ht="48">
       <c r="A25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8449,7 +8446,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="32" hidden="1">
+    <row r="26" spans="1:9" ht="32">
       <c r="A26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8482,7 +8479,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="48" hidden="1">
+    <row r="27" spans="1:9" ht="48">
       <c r="A27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8515,7 +8512,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="32" hidden="1">
+    <row r="28" spans="1:9" ht="32">
       <c r="A28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8548,7 +8545,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="48" hidden="1">
+    <row r="29" spans="1:9" ht="48">
       <c r="A29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8581,7 +8578,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="48" hidden="1">
+    <row r="30" spans="1:9" ht="48">
       <c r="A30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8614,7 +8611,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="48" hidden="1">
+    <row r="31" spans="1:9" ht="48">
       <c r="A31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8647,7 +8644,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="48" hidden="1">
+    <row r="32" spans="1:9" ht="48">
       <c r="A32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8680,7 +8677,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="48" hidden="1">
+    <row r="33" spans="1:9" ht="48">
       <c r="A33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8713,7 +8710,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="48" hidden="1">
+    <row r="34" spans="1:9" ht="48">
       <c r="A34" s="1" t="str">
         <f t="shared" ref="A34:A65" si="2">CONCATENATE("Population in TB compartment ",VLOOKUP(C34,TB_SET,2), " with ", VLOOKUP(D34,R_SET,2), " in HIV compartment ", VLOOKUP(E34,HIV_SET,2), " and ", VLOOKUP(F34, G_SET,2))</f>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -8746,7 +8743,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="48" hidden="1">
+    <row r="35" spans="1:9" ht="48">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -8778,7 +8775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="48" hidden="1">
+    <row r="36" spans="1:9" ht="48">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -8811,7 +8808,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="48" hidden="1">
+    <row r="37" spans="1:9" ht="48">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -8843,7 +8840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="48" hidden="1">
+    <row r="38" spans="1:9" ht="48">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -8909,7 +8906,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="48" hidden="1">
+    <row r="40" spans="1:9" ht="48">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -8942,7 +8939,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="48" hidden="1">
+    <row r="41" spans="1:9" ht="48">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -8975,7 +8972,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="32" hidden="1">
+    <row r="42" spans="1:9" ht="32">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9008,7 +9005,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="48" hidden="1">
+    <row r="43" spans="1:9" ht="48">
       <c r="A43" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9041,7 +9038,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="32" hidden="1">
+    <row r="44" spans="1:9" ht="32">
       <c r="A44" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9074,7 +9071,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="48" hidden="1">
+    <row r="45" spans="1:9" ht="48">
       <c r="A45" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9107,7 +9104,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="48" hidden="1">
+    <row r="46" spans="1:9" ht="48">
       <c r="A46" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9140,7 +9137,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="48" hidden="1">
+    <row r="47" spans="1:9" ht="48">
       <c r="A47" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9173,7 +9170,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="48" hidden="1">
+    <row r="48" spans="1:9" ht="48">
       <c r="A48" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9206,7 +9203,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="48" hidden="1">
+    <row r="49" spans="1:9" ht="48">
       <c r="A49" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9239,7 +9236,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="32" hidden="1">
+    <row r="50" spans="1:9" ht="32">
       <c r="A50" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9272,7 +9269,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="48" hidden="1">
+    <row r="51" spans="1:9" ht="48">
       <c r="A51" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -9304,7 +9301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="32" hidden="1">
+    <row r="52" spans="1:9" ht="32">
       <c r="A52" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9337,7 +9334,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="48" hidden="1">
+    <row r="53" spans="1:9" ht="48">
       <c r="A53" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -9369,7 +9366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="48" hidden="1">
+    <row r="54" spans="1:9" ht="48">
       <c r="A54" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9435,7 +9432,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="32" hidden="1">
+    <row r="56" spans="1:9" ht="32">
       <c r="A56" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9468,7 +9465,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="48" hidden="1">
+    <row r="57" spans="1:9" ht="48">
       <c r="A57" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9501,7 +9498,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="32" hidden="1">
+    <row r="58" spans="1:9" ht="32">
       <c r="A58" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9534,7 +9531,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="48" hidden="1">
+    <row r="59" spans="1:9" ht="48">
       <c r="A59" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9567,7 +9564,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="32" hidden="1">
+    <row r="60" spans="1:9" ht="32">
       <c r="A60" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9600,7 +9597,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="32" hidden="1">
+    <row r="61" spans="1:9" ht="32">
       <c r="A61" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9633,7 +9630,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="32" hidden="1">
+    <row r="62" spans="1:9" ht="32">
       <c r="A62" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9666,7 +9663,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="48" hidden="1">
+    <row r="63" spans="1:9" ht="48">
       <c r="A63" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9699,7 +9696,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="32" hidden="1">
+    <row r="64" spans="1:9" ht="32">
       <c r="A64" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9732,7 +9729,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="48" hidden="1">
+    <row r="65" spans="1:9" ht="48">
       <c r="A65" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9765,7 +9762,7 @@
         <v>327.38095238095326</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="32" hidden="1">
+    <row r="66" spans="1:9" ht="32">
       <c r="A66" s="1" t="str">
         <f t="shared" ref="A66:A97" si="4">CONCATENATE("Population in TB compartment ",VLOOKUP(C66,TB_SET,2), " with ", VLOOKUP(D66,R_SET,2), " in HIV compartment ", VLOOKUP(E66,HIV_SET,2), " and ", VLOOKUP(F66, G_SET,2))</f>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -9798,7 +9795,7 @@
         <v>2410.7142857142917</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="48" hidden="1">
+    <row r="67" spans="1:9" ht="48">
       <c r="A67" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -9830,7 +9827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="32" hidden="1">
+    <row r="68" spans="1:9" ht="32">
       <c r="A68" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -9863,7 +9860,7 @@
         <v>2410.7142857142917</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="48" hidden="1">
+    <row r="69" spans="1:9" ht="48">
       <c r="A69" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -9895,7 +9892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="48" hidden="1">
+    <row r="70" spans="1:9" ht="48">
       <c r="A70" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -9961,7 +9958,7 @@
         <v>2410.7142857142917</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="32" hidden="1">
+    <row r="72" spans="1:9" ht="32">
       <c r="A72" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -9994,7 +9991,7 @@
         <v>2410.7142857142917</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="48" hidden="1">
+    <row r="73" spans="1:9" ht="48">
       <c r="A73" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10027,7 +10024,7 @@
         <v>2410.7142857142917</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="32" hidden="1">
+    <row r="74" spans="1:9" ht="32">
       <c r="A74" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10060,7 +10057,7 @@
         <v>2410.7142857142917</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="32" hidden="1">
+    <row r="75" spans="1:9" ht="32">
       <c r="A75" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10093,7 +10090,7 @@
         <v>2410.7142857142917</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="32" hidden="1">
+    <row r="76" spans="1:9" ht="32">
       <c r="A76" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10126,7 +10123,7 @@
         <v>2410.7142857142917</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="32" hidden="1">
+    <row r="77" spans="1:9" ht="32">
       <c r="A77" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10159,7 +10156,7 @@
         <v>2410.7142857142917</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="32" hidden="1">
+    <row r="78" spans="1:9" ht="32">
       <c r="A78" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10192,7 +10189,7 @@
         <v>2410.7142857142917</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="48" hidden="1">
+    <row r="79" spans="1:9" ht="48">
       <c r="A79" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10225,7 +10222,7 @@
         <v>2410.7142857142917</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="32" hidden="1">
+    <row r="80" spans="1:9" ht="32">
       <c r="A80" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10258,7 +10255,7 @@
         <v>2410.7142857142917</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="32" hidden="1">
+    <row r="81" spans="1:9" ht="32">
       <c r="A81" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10291,7 +10288,7 @@
         <v>2410.7142857142917</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="48" hidden="1">
+    <row r="82" spans="1:9" ht="48">
       <c r="A82" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10324,7 +10321,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="48" hidden="1">
+    <row r="83" spans="1:9" ht="48">
       <c r="A83" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -10356,7 +10353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="48" hidden="1">
+    <row r="84" spans="1:9" ht="48">
       <c r="A84" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10389,7 +10386,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="48" hidden="1">
+    <row r="85" spans="1:9" ht="48">
       <c r="A85" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10421,7 +10418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="48" hidden="1">
+    <row r="86" spans="1:9" ht="48">
       <c r="A86" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10487,7 +10484,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="48" hidden="1">
+    <row r="88" spans="1:9" ht="48">
       <c r="A88" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10520,7 +10517,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="48" hidden="1">
+    <row r="89" spans="1:9" ht="48">
       <c r="A89" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10553,7 +10550,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="32" hidden="1">
+    <row r="90" spans="1:9" ht="32">
       <c r="A90" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10586,7 +10583,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="48" hidden="1">
+    <row r="91" spans="1:9" ht="48">
       <c r="A91" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10619,7 +10616,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="32" hidden="1">
+    <row r="92" spans="1:9" ht="32">
       <c r="A92" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10652,7 +10649,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="48" hidden="1">
+    <row r="93" spans="1:9" ht="48">
       <c r="A93" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10685,7 +10682,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="48" hidden="1">
+    <row r="94" spans="1:9" ht="48">
       <c r="A94" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10718,7 +10715,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="48" hidden="1">
+    <row r="95" spans="1:9" ht="48">
       <c r="A95" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10751,7 +10748,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="48" hidden="1">
+    <row r="96" spans="1:9" ht="48">
       <c r="A96" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10784,7 +10781,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="48" hidden="1">
+    <row r="97" spans="1:9" ht="48">
       <c r="A97" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10817,7 +10814,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="48" hidden="1">
+    <row r="98" spans="1:9" ht="48">
       <c r="A98" s="1" t="str">
         <f t="shared" ref="A98:A129" si="6">CONCATENATE("Population in TB compartment ",VLOOKUP(C98,TB_SET,2), " with ", VLOOKUP(D98,R_SET,2), " in HIV compartment ", VLOOKUP(E98,HIV_SET,2), " and ", VLOOKUP(F98, G_SET,2))</f>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -10850,7 +10847,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="48" hidden="1">
+    <row r="99" spans="1:9" ht="48">
       <c r="A99" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10882,7 +10879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="48" hidden="1">
+    <row r="100" spans="1:9" ht="48">
       <c r="A100" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -10915,7 +10912,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="48" hidden="1">
+    <row r="101" spans="1:9" ht="48">
       <c r="A101" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10947,7 +10944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="48" hidden="1">
+    <row r="102" spans="1:9" ht="48">
       <c r="A102" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11013,7 +11010,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="48" hidden="1">
+    <row r="104" spans="1:9" ht="48">
       <c r="A104" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11046,7 +11043,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="48" hidden="1">
+    <row r="105" spans="1:9" ht="48">
       <c r="A105" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11079,7 +11076,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="32" hidden="1">
+    <row r="106" spans="1:9" ht="32">
       <c r="A106" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11112,7 +11109,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="48" hidden="1">
+    <row r="107" spans="1:9" ht="48">
       <c r="A107" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11145,7 +11142,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="32" hidden="1">
+    <row r="108" spans="1:9" ht="32">
       <c r="A108" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11178,7 +11175,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="48" hidden="1">
+    <row r="109" spans="1:9" ht="48">
       <c r="A109" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11211,7 +11208,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="48" hidden="1">
+    <row r="110" spans="1:9" ht="48">
       <c r="A110" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11244,7 +11241,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="48" hidden="1">
+    <row r="111" spans="1:9" ht="48">
       <c r="A111" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11277,7 +11274,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="48" hidden="1">
+    <row r="112" spans="1:9" ht="48">
       <c r="A112" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11310,7 +11307,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="48" hidden="1">
+    <row r="113" spans="1:9" ht="48">
       <c r="A113" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11343,7 +11340,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="48" hidden="1">
+    <row r="114" spans="1:9" ht="48">
       <c r="A114" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11376,7 +11373,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="48" hidden="1">
+    <row r="115" spans="1:9" ht="48">
       <c r="A115" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11408,7 +11405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="48" hidden="1">
+    <row r="116" spans="1:9" ht="48">
       <c r="A116" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11441,7 +11438,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="48" hidden="1">
+    <row r="117" spans="1:9" ht="48">
       <c r="A117" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11473,7 +11470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="48" hidden="1">
+    <row r="118" spans="1:9" ht="48">
       <c r="A118" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11539,7 +11536,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="48" hidden="1">
+    <row r="120" spans="1:9" ht="48">
       <c r="A120" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11572,7 +11569,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="48" hidden="1">
+    <row r="121" spans="1:9" ht="48">
       <c r="A121" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11605,7 +11602,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="32" hidden="1">
+    <row r="122" spans="1:9" ht="32">
       <c r="A122" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11638,7 +11635,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="48" hidden="1">
+    <row r="123" spans="1:9" ht="48">
       <c r="A123" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11671,7 +11668,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="32" hidden="1">
+    <row r="124" spans="1:9" ht="32">
       <c r="A124" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11704,7 +11701,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="32" hidden="1">
+    <row r="125" spans="1:9" ht="32">
       <c r="A125" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11737,7 +11734,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="48" hidden="1">
+    <row r="126" spans="1:9" ht="48">
       <c r="A126" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11770,7 +11767,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="48" hidden="1">
+    <row r="127" spans="1:9" ht="48">
       <c r="A127" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11803,7 +11800,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="48" hidden="1">
+    <row r="128" spans="1:9" ht="48">
       <c r="A128" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11836,7 +11833,7 @@
         <v>267.85714285714357</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="48" hidden="1">
+    <row r="129" spans="1:9" ht="48">
       <c r="A129" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12126,18 +12123,6 @@
       <c r="C194" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L129" xr:uid="{6FA4CCEF-026B-E44B-89F3-D945F0CFA0FA}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="3"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters>
-        <filter val="2"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <sortState ref="A2:L129">
     <sortCondition ref="F2:F129"/>
   </sortState>
@@ -12153,7 +12138,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
update epi param file rho into 5 (incorrectO -->6 (correct)
</commit_message>
<xml_diff>
--- a/param_files/Epi_parameters_June_24_2020.xlsx
+++ b/param_files/Epi_parameters_June_24_2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jross3\Repos\k01\epi_model_HIV_TB\param_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/GitHub/epi_model_HIV_TB/param_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA349A2-841F-423C-8734-5ECB45D36951}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274B8C43-C6CB-F948-9BDF-F1F135E1FF6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Matched_Parameters" sheetId="1" r:id="rId1"/>
@@ -27,18 +27,10 @@
     <definedName name="R_SET">'Set Ref'!$A$11:$B$13</definedName>
     <definedName name="TB_SET">'Set Ref'!$A$1:$B$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1508,34 +1500,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:O194"/>
   <sheetViews>
-    <sheetView zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="K136" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <pane xSplit="10" ySplit="1" topLeftCell="K179" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K102" sqref="K102"/>
+      <selection pane="bottomRight" activeCell="K188" sqref="K188"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="69.33203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="53" style="9" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="7.796875" style="9" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="7.83203125" style="9" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="9" hidden="1" customWidth="1"/>
     <col min="6" max="7" width="15" style="9" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="26" style="9" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" style="9" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" style="9" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="9" customWidth="1"/>
-    <col min="12" max="12" width="17.796875" style="9" customWidth="1"/>
-    <col min="13" max="13" width="20.46484375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="20.5" style="9" customWidth="1"/>
     <col min="14" max="14" width="28.6640625" style="9" customWidth="1"/>
     <col min="15" max="15" width="29" style="10" customWidth="1"/>
-    <col min="16" max="16384" width="8.796875" style="10"/>
+    <col min="16" max="16384" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="7" customFormat="1" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1582,7 +1575,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>15</v>
       </c>
@@ -1610,7 +1603,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>19</v>
       </c>
@@ -1638,7 +1631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>20</v>
       </c>
@@ -1666,7 +1659,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>23</v>
       </c>
@@ -1694,7 +1687,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>24</v>
       </c>
@@ -1722,7 +1715,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>27</v>
       </c>
@@ -1750,7 +1743,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>28</v>
       </c>
@@ -1781,7 +1774,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>32</v>
       </c>
@@ -1813,7 +1806,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>33</v>
       </c>
@@ -1845,7 +1838,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>34</v>
       </c>
@@ -1877,7 +1870,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>35</v>
       </c>
@@ -1905,7 +1898,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>39</v>
       </c>
@@ -1927,7 +1920,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>41</v>
       </c>
@@ -1964,7 +1957,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>45</v>
       </c>
@@ -2001,7 +1994,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>46</v>
       </c>
@@ -2041,7 +2034,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>49</v>
       </c>
@@ -2081,7 +2074,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>50</v>
       </c>
@@ -2121,7 +2114,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>51</v>
       </c>
@@ -2161,7 +2154,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>52</v>
       </c>
@@ -2201,7 +2194,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>53</v>
       </c>
@@ -2241,7 +2234,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>54</v>
       </c>
@@ -2278,7 +2271,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>55</v>
       </c>
@@ -2315,7 +2308,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>56</v>
       </c>
@@ -2355,7 +2348,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>58</v>
       </c>
@@ -2395,7 +2388,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
         <v>59</v>
       </c>
@@ -2435,7 +2428,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>60</v>
       </c>
@@ -2475,7 +2468,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
         <v>61</v>
       </c>
@@ -2512,7 +2505,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>62</v>
       </c>
@@ -2549,7 +2542,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
         <v>63</v>
       </c>
@@ -2586,7 +2579,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
         <v>64</v>
       </c>
@@ -2623,7 +2616,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
         <v>65</v>
       </c>
@@ -2660,7 +2653,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
         <v>66</v>
       </c>
@@ -2697,7 +2690,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
         <v>67</v>
       </c>
@@ -2734,7 +2727,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
         <v>68</v>
       </c>
@@ -2771,7 +2764,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
         <v>69</v>
       </c>
@@ -2808,7 +2801,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
         <v>70</v>
       </c>
@@ -2845,7 +2838,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
         <v>71</v>
       </c>
@@ -2882,7 +2875,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
         <v>73</v>
       </c>
@@ -2919,7 +2912,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
         <v>74</v>
       </c>
@@ -2959,7 +2952,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
         <v>76</v>
       </c>
@@ -2999,7 +2992,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
         <v>77</v>
       </c>
@@ -3039,7 +3032,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
         <v>78</v>
       </c>
@@ -3079,7 +3072,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
         <v>79</v>
       </c>
@@ -3119,7 +3112,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
         <v>80</v>
       </c>
@@ -3159,7 +3152,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
         <v>81</v>
       </c>
@@ -3199,7 +3192,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
         <v>82</v>
       </c>
@@ -3239,7 +3232,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
         <v>83</v>
       </c>
@@ -3276,7 +3269,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
         <v>84</v>
       </c>
@@ -3313,7 +3306,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
         <v>85</v>
       </c>
@@ -3350,7 +3343,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
         <v>86</v>
       </c>
@@ -3387,7 +3380,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
         <v>87</v>
       </c>
@@ -3424,7 +3417,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
         <v>88</v>
       </c>
@@ -3461,7 +3454,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
         <v>89</v>
       </c>
@@ -3498,7 +3491,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
         <v>91</v>
       </c>
@@ -3535,7 +3528,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
         <v>92</v>
       </c>
@@ -3572,7 +3565,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
         <v>93</v>
       </c>
@@ -3609,7 +3602,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
         <v>94</v>
       </c>
@@ -3646,7 +3639,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
         <v>95</v>
       </c>
@@ -3683,7 +3676,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
         <v>96</v>
       </c>
@@ -3720,7 +3713,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="20" t="s">
         <v>97</v>
       </c>
@@ -3757,7 +3750,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
         <v>98</v>
       </c>
@@ -3794,7 +3787,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
         <v>99</v>
       </c>
@@ -3831,7 +3824,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
         <v>100</v>
       </c>
@@ -3868,7 +3861,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
         <v>101</v>
       </c>
@@ -3905,7 +3898,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
         <v>102</v>
       </c>
@@ -3942,7 +3935,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
         <v>103</v>
       </c>
@@ -3979,7 +3972,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
         <v>104</v>
       </c>
@@ -4016,7 +4009,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
         <v>105</v>
       </c>
@@ -4053,7 +4046,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="20" t="s">
         <v>106</v>
       </c>
@@ -4090,7 +4083,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="20" t="s">
         <v>107</v>
       </c>
@@ -4127,7 +4120,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="s">
         <v>108</v>
       </c>
@@ -4164,7 +4157,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="20" t="s">
         <v>109</v>
       </c>
@@ -4201,7 +4194,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="20" t="s">
         <v>110</v>
       </c>
@@ -4238,7 +4231,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="s">
         <v>111</v>
       </c>
@@ -4275,7 +4268,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="20" t="s">
         <v>112</v>
       </c>
@@ -4312,7 +4305,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="20" t="s">
         <v>113</v>
       </c>
@@ -4349,7 +4342,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="20" t="s">
         <v>114</v>
       </c>
@@ -4386,7 +4379,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="20" t="s">
         <v>115</v>
       </c>
@@ -4423,7 +4416,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="20" t="s">
         <v>116</v>
       </c>
@@ -4460,7 +4453,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="20" t="s">
         <v>117</v>
       </c>
@@ -4497,7 +4490,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="20" t="s">
         <v>118</v>
       </c>
@@ -4534,7 +4527,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="63" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="20" t="s">
         <v>119</v>
       </c>
@@ -4571,7 +4564,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="20" t="s">
         <v>120</v>
       </c>
@@ -4608,7 +4601,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="20" t="s">
         <v>121</v>
       </c>
@@ -4645,7 +4638,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="20" t="s">
         <v>122</v>
       </c>
@@ -4670,7 +4663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="20" t="s">
         <v>122</v>
       </c>
@@ -4695,7 +4688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="20" t="s">
         <v>124</v>
       </c>
@@ -4726,7 +4719,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="20" t="s">
         <v>127</v>
       </c>
@@ -4757,7 +4750,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="20" t="s">
         <v>128</v>
       </c>
@@ -4788,7 +4781,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="20" t="s">
         <v>129</v>
       </c>
@@ -4819,7 +4812,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="20" t="s">
         <v>130</v>
       </c>
@@ -4850,7 +4843,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="20" t="s">
         <v>131</v>
       </c>
@@ -4881,7 +4874,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="20" t="s">
         <v>132</v>
       </c>
@@ -4908,7 +4901,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="20" t="s">
         <v>136</v>
       </c>
@@ -4932,7 +4925,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="20" t="s">
         <v>137</v>
       </c>
@@ -4956,7 +4949,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="20" t="s">
         <v>138</v>
       </c>
@@ -4980,7 +4973,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="20" t="s">
         <v>139</v>
       </c>
@@ -5006,7 +4999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="20" t="s">
         <v>141</v>
       </c>
@@ -5032,7 +5025,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="20" t="s">
         <v>142</v>
       </c>
@@ -5058,7 +5051,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="20" t="s">
         <v>143</v>
       </c>
@@ -5084,7 +5077,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="22" t="s">
         <v>274</v>
       </c>
@@ -5108,7 +5101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="20" t="s">
         <v>144</v>
       </c>
@@ -5140,7 +5133,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="20" t="s">
         <v>148</v>
       </c>
@@ -5172,7 +5165,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="20" t="s">
         <v>150</v>
       </c>
@@ -5205,7 +5198,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="20" t="s">
         <v>152</v>
       </c>
@@ -5238,7 +5231,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="20" t="s">
         <v>154</v>
       </c>
@@ -5270,7 +5263,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="20" t="s">
         <v>156</v>
       </c>
@@ -5299,7 +5292,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="20" t="s">
         <v>157</v>
       </c>
@@ -5329,7 +5322,7 @@
         <v>0.22000000000000003</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="20" t="s">
         <v>158</v>
       </c>
@@ -5359,7 +5352,7 @@
         <v>0.44000000000000006</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="20" t="s">
         <v>159</v>
       </c>
@@ -5388,7 +5381,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="20" t="s">
         <v>160</v>
       </c>
@@ -5417,7 +5410,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:11" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="20" t="s">
         <v>161</v>
       </c>
@@ -5446,7 +5439,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:11" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="20" t="s">
         <v>162</v>
       </c>
@@ -5475,7 +5468,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="20" t="s">
         <v>163</v>
       </c>
@@ -5506,7 +5499,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="20" t="s">
         <v>166</v>
       </c>
@@ -5537,7 +5530,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="20" t="s">
         <v>167</v>
       </c>
@@ -5569,7 +5562,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="20" t="s">
         <v>168</v>
       </c>
@@ -5601,7 +5594,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="20" t="s">
         <v>169</v>
       </c>
@@ -5633,7 +5626,7 @@
         <v>2.2050000000000004E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="20" t="s">
         <v>170</v>
       </c>
@@ -5665,7 +5658,7 @@
         <v>2.2050000000000004E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="20" t="s">
         <v>171</v>
       </c>
@@ -5697,7 +5690,7 @@
         <v>2.3152500000000006E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="20" t="s">
         <v>172</v>
       </c>
@@ -5729,7 +5722,7 @@
         <v>2.3152500000000006E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="20" t="s">
         <v>173</v>
       </c>
@@ -5761,7 +5754,7 @@
         <v>2.2000000000000002E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="20" t="s">
         <v>174</v>
       </c>
@@ -5793,7 +5786,7 @@
         <v>2.2000000000000002E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="20" t="s">
         <v>175</v>
       </c>
@@ -5825,7 +5818,7 @@
         <v>2.3100000000000002E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="20" t="s">
         <v>176</v>
       </c>
@@ -5857,7 +5850,7 @@
         <v>2.3100000000000002E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="20" t="s">
         <v>177</v>
       </c>
@@ -5889,7 +5882,7 @@
         <v>2.5410000000000005E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="20" t="s">
         <v>178</v>
       </c>
@@ -5921,7 +5914,7 @@
         <v>2.5410000000000005E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="20" t="s">
         <v>179</v>
       </c>
@@ -5953,7 +5946,7 @@
         <v>2.7951000000000007E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="20" t="s">
         <v>180</v>
       </c>
@@ -5985,7 +5978,7 @@
         <v>2.7951000000000007E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="20" t="s">
         <v>181</v>
       </c>
@@ -6016,7 +6009,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="20" t="s">
         <v>182</v>
       </c>
@@ -6048,7 +6041,7 @@
         <v>3.0746100000000009E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="20" t="s">
         <v>183</v>
       </c>
@@ -6080,7 +6073,7 @@
         <v>2.2000000000000002E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="20" t="s">
         <v>184</v>
       </c>
@@ -6112,7 +6105,7 @@
         <v>3.3820710000000011E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="20" t="s">
         <v>185</v>
       </c>
@@ -6144,7 +6137,7 @@
         <v>2.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="20" t="s">
         <v>186</v>
       </c>
@@ -6176,7 +6169,7 @@
         <v>3.7202781000000018E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="20" t="s">
         <v>187</v>
       </c>
@@ -6208,7 +6201,7 @@
         <v>2.6620000000000005E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="20" t="s">
         <v>188</v>
       </c>
@@ -6240,7 +6233,7 @@
         <v>4.092305910000002E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="20" t="s">
         <v>189</v>
       </c>
@@ -6272,7 +6265,7 @@
         <v>2.9282000000000006E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="20" t="s">
         <v>190</v>
       </c>
@@ -6304,7 +6297,7 @@
         <v>4.5015365010000023E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="20" t="s">
         <v>191</v>
       </c>
@@ -6336,7 +6329,7 @@
         <v>3.2210200000000008E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="20" t="s">
         <v>192</v>
       </c>
@@ -6368,7 +6361,7 @@
         <v>4.9516901511000029E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="20" t="s">
         <v>193</v>
       </c>
@@ -6400,7 +6393,7 @@
         <v>3.5431220000000013E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="20" t="s">
         <v>194</v>
       </c>
@@ -6432,7 +6425,7 @@
         <v>5.4468591662100038E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="20" t="s">
         <v>195</v>
       </c>
@@ -6464,7 +6457,7 @@
         <v>3.8974342000000016E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="20" t="s">
         <v>196</v>
       </c>
@@ -6496,7 +6489,7 @@
         <v>5.9915450828310048E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="20" t="s">
         <v>197</v>
       </c>
@@ -6528,7 +6521,7 @@
         <v>4.092305910000002E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="20" t="s">
         <v>198</v>
       </c>
@@ -6560,7 +6553,7 @@
         <v>6.2911223369725558E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="20" t="s">
         <v>199</v>
       </c>
@@ -6592,7 +6585,7 @@
         <v>4.2969212055000025E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="20" t="s">
         <v>200</v>
       </c>
@@ -6624,7 +6617,7 @@
         <v>6.9202345706698115E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="20" t="s">
         <v>201</v>
       </c>
@@ -6656,7 +6649,7 @@
         <v>4.7266133260500033E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="20" t="s">
         <v>202</v>
       </c>
@@ -6688,7 +6681,7 @@
         <v>7.6122580277367929E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="20" t="s">
         <v>203</v>
       </c>
@@ -6720,7 +6713,7 @@
         <v>5.1992746586550044E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="20" t="s">
         <v>204</v>
       </c>
@@ -6752,7 +6745,7 @@
         <v>8.3734838305104725E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="20" t="s">
         <v>205</v>
       </c>
@@ -6784,7 +6777,7 @@
         <v>6.7590570562515065E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="20" t="s">
         <v>206</v>
       </c>
@@ -6816,7 +6809,7 @@
         <v>0.10885528979663614</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="20" t="s">
         <v>207</v>
       </c>
@@ -6848,7 +6841,7 @@
         <v>8.7867741731269586E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="20" t="s">
         <v>208</v>
       </c>
@@ -6880,7 +6873,7 @@
         <v>0.14151187673562698</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="20" t="s">
         <v>209</v>
       </c>
@@ -6912,7 +6905,7 @@
         <v>0.11422806425065046</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="20" t="s">
         <v>210</v>
       </c>
@@ -6944,7 +6937,7 @@
         <v>0.18396543975631507</v>
       </c>
     </row>
-    <row r="161" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="20" t="s">
         <v>211</v>
       </c>
@@ -6976,7 +6969,7 @@
         <v>0.1484964835258456</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="20" t="s">
         <v>212</v>
       </c>
@@ -7008,7 +7001,7 @@
         <v>0.2391550716832096</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="20" t="s">
         <v>213</v>
       </c>
@@ -7040,7 +7033,7 @@
         <v>0.11879718682067648</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="20" t="s">
         <v>214</v>
       </c>
@@ -7072,7 +7065,7 @@
         <v>0.19132405734656768</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="20" t="s">
         <v>215</v>
       </c>
@@ -7104,7 +7097,7 @@
         <v>9.5037749456541198E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="20" t="s">
         <v>216</v>
       </c>
@@ -7136,7 +7129,7 @@
         <v>0.15305924587725417</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="20" t="s">
         <v>217</v>
       </c>
@@ -7168,7 +7161,7 @@
         <v>7.6030199565232964E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="20" t="s">
         <v>218</v>
       </c>
@@ -7200,7 +7193,7 @@
         <v>0.12244739670180334</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="20" t="s">
         <v>219</v>
       </c>
@@ -7232,7 +7225,7 @@
         <v>6.0824159652186377E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="20" t="s">
         <v>220</v>
       </c>
@@ -7264,7 +7257,7 @@
         <v>9.7957917361442673E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="20" t="s">
         <v>221</v>
       </c>
@@ -7296,7 +7289,7 @@
         <v>4.2576911756530458E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="20" t="s">
         <v>222</v>
       </c>
@@ -7328,7 +7321,7 @@
         <v>6.8570542153009867E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="20" t="s">
         <v>223</v>
       </c>
@@ -7360,7 +7353,7 @@
         <v>2.9803838229571319E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="20" t="s">
         <v>224</v>
       </c>
@@ -7392,7 +7385,7 @@
         <v>4.7999379507106907E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="20" t="s">
         <v>225</v>
       </c>
@@ -7424,7 +7417,7 @@
         <v>2.0862686760699922E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="20" t="s">
         <v>226</v>
       </c>
@@ -7456,7 +7449,7 @@
         <v>3.3599565654974829E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="20" t="s">
         <v>227</v>
       </c>
@@ -7488,7 +7481,7 @@
         <v>1.4603880732489943E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="20" t="s">
         <v>228</v>
       </c>
@@ -7520,7 +7513,7 @@
         <v>2.351969595848238E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A179" s="20" t="s">
         <v>229</v>
       </c>
@@ -7551,7 +7544,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A180" s="20" t="s">
         <v>229</v>
       </c>
@@ -7582,7 +7575,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A181" s="20" t="s">
         <v>229</v>
       </c>
@@ -7613,7 +7606,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A182" s="20" t="s">
         <v>229</v>
       </c>
@@ -7628,7 +7621,7 @@
         <v>165</v>
       </c>
       <c r="E182" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G182" s="9">
         <v>1</v>
@@ -7638,13 +7631,13 @@
       </c>
       <c r="J182" s="9" t="str">
         <f t="shared" si="15"/>
-        <v>rho_5,1,1</v>
+        <v>rho_6,1,1</v>
       </c>
       <c r="K182" s="23">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A183" s="20" t="s">
         <v>231</v>
       </c>
@@ -7676,7 +7669,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="184" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A184" s="20" t="s">
         <v>231</v>
       </c>
@@ -7708,7 +7701,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="185" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A185" s="20" t="s">
         <v>231</v>
       </c>
@@ -7740,7 +7733,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="186" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A186" s="20" t="s">
         <v>231</v>
       </c>
@@ -7755,7 +7748,7 @@
         <v>165</v>
       </c>
       <c r="E186" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G186" s="9">
         <v>2</v>
@@ -7765,14 +7758,14 @@
       </c>
       <c r="J186" s="9" t="str">
         <f t="shared" si="15"/>
-        <v>rho_5,2,1</v>
+        <v>rho_6,2,1</v>
       </c>
       <c r="K186" s="23">
         <f t="shared" si="19"/>
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="187" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A187" s="20" t="s">
         <v>232</v>
       </c>
@@ -7804,7 +7797,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A188" s="20" t="s">
         <v>232</v>
       </c>
@@ -7836,7 +7829,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="189" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A189" s="20" t="s">
         <v>232</v>
       </c>
@@ -7868,7 +7861,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="190" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A190" s="20" t="s">
         <v>232</v>
       </c>
@@ -7883,7 +7876,7 @@
         <v>165</v>
       </c>
       <c r="E190" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G190" s="9">
         <v>1</v>
@@ -7893,14 +7886,14 @@
       </c>
       <c r="J190" s="9" t="str">
         <f t="shared" si="15"/>
-        <v>rho_5,1,2</v>
+        <v>rho_6,1,2</v>
       </c>
       <c r="K190" s="23">
         <f t="shared" si="20"/>
         <v>4.7499999999999999E-3</v>
       </c>
     </row>
-    <row r="191" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A191" s="20" t="s">
         <v>233</v>
       </c>
@@ -7932,7 +7925,7 @@
         <v>1.9000000000000001E-4</v>
       </c>
     </row>
-    <row r="192" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A192" s="20" t="s">
         <v>233</v>
       </c>
@@ -7964,7 +7957,7 @@
         <v>9.5000000000000005E-5</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A193" s="20" t="s">
         <v>233</v>
       </c>
@@ -7996,7 +7989,7 @@
         <v>9.5000000000000005E-5</v>
       </c>
     </row>
-    <row r="194" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A194" s="20" t="s">
         <v>233</v>
       </c>
@@ -8011,7 +8004,7 @@
         <v>165</v>
       </c>
       <c r="E194" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G194" s="9">
         <v>2</v>
@@ -8020,8 +8013,8 @@
         <v>2</v>
       </c>
       <c r="J194" s="9" t="str">
-        <f t="shared" ref="J194:J225" si="21">CONCATENATE(C194, "_", E194, IF(E194&lt;&gt;"",",",""), F194, IF(F194&lt;&gt;"",",",""),  G194, IF(G194&lt;&gt;"",",",""),  H194, IF(I194&lt;&gt;"","(",""), I194, IF(I194&lt;&gt;"",")",""))</f>
-        <v>rho_5,2,2</v>
+        <f t="shared" ref="J194" si="21">CONCATENATE(C194, "_", E194, IF(E194&lt;&gt;"",",",""), F194, IF(F194&lt;&gt;"",",",""),  G194, IF(G194&lt;&gt;"",",",""),  H194, IF(I194&lt;&gt;"","(",""), I194, IF(I194&lt;&gt;"",")",""))</f>
+        <v>rho_6,2,2</v>
       </c>
       <c r="K194" s="23">
         <f t="shared" si="20"/>
@@ -8029,7 +8022,14 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O194">
+  <autoFilter ref="A1:O194" xr:uid="{BC67A81D-7C1F-3D4A-875A-F60944DEF322}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="rho"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A2:O194">
     <sortCondition ref="D2:D194"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8046,21 +8046,21 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.1328125" customWidth="1"/>
+    <col min="1" max="1" width="52.1640625" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="9" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="9" hidden="1" customWidth="1"/>
     <col min="4" max="5" width="15" style="9" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="26" style="9" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="22.33203125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="17.46484375" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.46484375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.796875" style="1" customWidth="1"/>
-    <col min="11" max="12" width="20.46484375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="20.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>276</v>
       </c>
@@ -8098,7 +8098,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
         <f t="shared" ref="A2:A33" si="0">CONCATENATE("Population in TB compartment ",VLOOKUP(C2,TB_SET,2), " with ", VLOOKUP(D2,R_SET,2), " in HIV compartment ", VLOOKUP(E2,HIV_SET,2), " and ", VLOOKUP(F2, G_SET,2))</f>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8130,7 +8130,7 @@
         <v>32693.093583980408</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8162,7 +8162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8195,7 +8195,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8227,7 +8227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8260,7 +8260,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8293,7 +8293,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8326,7 +8326,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8359,7 +8359,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8392,7 +8392,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8425,7 +8425,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8458,7 +8458,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8491,7 +8491,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8524,7 +8524,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8557,7 +8557,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8590,7 +8590,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8623,7 +8623,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8656,7 +8656,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -8688,7 +8688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8721,7 +8721,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -8753,7 +8753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8786,7 +8786,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8819,7 +8819,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8852,7 +8852,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8885,7 +8885,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8918,7 +8918,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8951,7 +8951,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8984,7 +8984,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -9017,7 +9017,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -9050,7 +9050,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -9083,7 +9083,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -9116,7 +9116,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -9149,7 +9149,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="str">
         <f t="shared" ref="A34:A65" si="2">CONCATENATE("Population in TB compartment ",VLOOKUP(C34,TB_SET,2), " with ", VLOOKUP(D34,R_SET,2), " in HIV compartment ", VLOOKUP(E34,HIV_SET,2), " and ", VLOOKUP(F34, G_SET,2))</f>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9182,7 +9182,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -9214,7 +9214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9247,7 +9247,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -9279,7 +9279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9312,7 +9312,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9345,7 +9345,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9378,7 +9378,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9411,7 +9411,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9444,7 +9444,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9477,7 +9477,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9510,7 +9510,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9543,7 +9543,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9576,7 +9576,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9609,7 +9609,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9642,7 +9642,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9675,7 +9675,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9708,7 +9708,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -9740,7 +9740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9773,7 +9773,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -9805,7 +9805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9838,7 +9838,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9871,7 +9871,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9904,7 +9904,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9937,7 +9937,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9970,7 +9970,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10003,7 +10003,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10036,7 +10036,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10069,7 +10069,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10102,7 +10102,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10135,7 +10135,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10168,7 +10168,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10201,7 +10201,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="str">
         <f t="shared" ref="A66:A97" si="4">CONCATENATE("Population in TB compartment ",VLOOKUP(C66,TB_SET,2), " with ", VLOOKUP(D66,R_SET,2), " in HIV compartment ", VLOOKUP(E66,HIV_SET,2), " and ", VLOOKUP(F66, G_SET,2))</f>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10234,7 +10234,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -10266,7 +10266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10299,7 +10299,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -10331,7 +10331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10364,7 +10364,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10397,7 +10397,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10430,7 +10430,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10463,7 +10463,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10496,7 +10496,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10529,7 +10529,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10562,7 +10562,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10595,7 +10595,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10628,7 +10628,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10661,7 +10661,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10694,7 +10694,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10727,7 +10727,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10760,7 +10760,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -10792,7 +10792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10825,7 +10825,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10857,7 +10857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10890,7 +10890,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10923,7 +10923,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10956,7 +10956,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10989,7 +10989,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11022,7 +11022,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11055,7 +11055,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11088,7 +11088,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11121,7 +11121,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11154,7 +11154,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11187,7 +11187,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11220,7 +11220,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11253,7 +11253,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="str">
         <f t="shared" ref="A98:A129" si="6">CONCATENATE("Population in TB compartment ",VLOOKUP(C98,TB_SET,2), " with ", VLOOKUP(D98,R_SET,2), " in HIV compartment ", VLOOKUP(E98,HIV_SET,2), " and ", VLOOKUP(F98, G_SET,2))</f>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11286,7 +11286,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -11318,7 +11318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11351,7 +11351,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11383,7 +11383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11416,7 +11416,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11449,7 +11449,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11482,7 +11482,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11515,7 +11515,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11548,7 +11548,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11581,7 +11581,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11614,7 +11614,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11647,7 +11647,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11680,7 +11680,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11713,7 +11713,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11746,7 +11746,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11779,7 +11779,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11812,7 +11812,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11844,7 +11844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11877,7 +11877,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11909,7 +11909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11942,7 +11942,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11975,7 +11975,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12008,7 +12008,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12041,7 +12041,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12074,7 +12074,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12107,7 +12107,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12140,7 +12140,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12173,7 +12173,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12206,7 +12206,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12239,7 +12239,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12272,7 +12272,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12305,264 +12305,264 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B144" s="8"/>
       <c r="C144" s="8"/>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B145" s="8"/>
       <c r="C145" s="8"/>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B148" s="8"/>
       <c r="C148" s="8"/>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B149" s="8"/>
       <c r="C149" s="8"/>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="160" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B161" s="8"/>
       <c r="C161" s="8"/>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="163" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B163" s="8"/>
       <c r="C163" s="8"/>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B164" s="8"/>
       <c r="C164" s="8"/>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B165" s="8"/>
       <c r="C165" s="8"/>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B166" s="8"/>
       <c r="C166" s="8"/>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="167" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B167" s="8"/>
       <c r="C167" s="8"/>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="169" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B169" s="8"/>
       <c r="C169" s="8"/>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="170" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="171" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B171" s="8"/>
       <c r="C171" s="8"/>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="172" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B172" s="8"/>
       <c r="C172" s="8"/>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="173" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B173" s="8"/>
       <c r="C173" s="8"/>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="174" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B174" s="8"/>
       <c r="C174" s="8"/>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B175" s="8"/>
       <c r="C175" s="8"/>
     </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="176" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="177" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="178" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
     </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="179" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B179" s="8"/>
       <c r="C179" s="8"/>
     </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="180" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B180" s="8"/>
       <c r="C180" s="8"/>
     </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="181" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B181" s="8"/>
       <c r="C181" s="8"/>
     </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="182" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B182" s="8"/>
       <c r="C182" s="8"/>
     </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="183" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B183" s="8"/>
       <c r="C183" s="8"/>
     </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="184" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B184" s="8"/>
       <c r="C184" s="8"/>
     </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="185" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B185" s="8"/>
       <c r="C185" s="8"/>
     </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="187" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B187" s="8"/>
       <c r="C187" s="8"/>
     </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="188" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B188" s="8"/>
       <c r="C188" s="8"/>
     </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="189" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B189" s="8"/>
       <c r="C189" s="8"/>
     </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="190" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B190" s="8"/>
       <c r="C190" s="8"/>
     </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="191" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B191" s="8"/>
       <c r="C191" s="8"/>
     </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="192" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B192" s="8"/>
       <c r="C192" s="8"/>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="193" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B193" s="8"/>
       <c r="C193" s="8"/>
     </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="194" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B194" s="8"/>
       <c r="C194" s="8"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L129">
+  <sortState ref="A2:L129">
     <sortCondition ref="F2:F129"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12573,26 +12573,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD4AF83-5BDA-B246-9A8F-C4F47C31E1D4}">
   <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B108352" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
+      <selection pane="bottomRight" activeCell="C111481" sqref="C111481"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.46484375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.796875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="20.46484375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.46484375" customWidth="1"/>
-    <col min="8" max="8" width="15.46484375" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="8.796875" style="4"/>
+    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="20.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.5" customWidth="1"/>
+    <col min="8" max="8" width="15.5" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -12618,7 +12618,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>237</v>
       </c>
@@ -12629,7 +12629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>239</v>
       </c>
@@ -12640,7 +12640,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>241</v>
       </c>
@@ -12651,7 +12651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>243</v>
       </c>
@@ -12662,7 +12662,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>243</v>
       </c>
@@ -12673,7 +12673,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>243</v>
       </c>
@@ -12684,7 +12684,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>243</v>
       </c>
@@ -12695,7 +12695,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>248</v>
       </c>
@@ -12706,7 +12706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>277</v>
       </c>
@@ -12714,7 +12714,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>278</v>
       </c>
@@ -12722,7 +12722,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
         <v>279</v>
       </c>
@@ -12730,7 +12730,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
         <v>280</v>
       </c>
@@ -12738,7 +12738,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
         <v>282</v>
       </c>
@@ -12746,12 +12746,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
         <v>298</v>
       </c>
@@ -12759,280 +12759,280 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
         <v>299</v>
       </c>
       <c r="H17" s="31"/>
     </row>
-    <row r="18" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
         <v>284</v>
       </c>
       <c r="H18" s="31"/>
     </row>
-    <row r="19" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>285</v>
       </c>
       <c r="H19" s="31"/>
     </row>
-    <row r="20" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
         <v>286</v>
       </c>
       <c r="H20" s="31"/>
     </row>
-    <row r="21" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
         <v>287</v>
       </c>
       <c r="H21" s="31"/>
     </row>
-    <row r="22" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
         <v>288</v>
       </c>
       <c r="H22" s="31"/>
     </row>
-    <row r="23" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="s">
         <v>289</v>
       </c>
       <c r="H23" s="31"/>
     </row>
-    <row r="24" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
         <v>290</v>
       </c>
       <c r="H24" s="31"/>
     </row>
-    <row r="25" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="27" t="s">
         <v>291</v>
       </c>
       <c r="H25" s="31"/>
     </row>
-    <row r="26" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="27" t="s">
         <v>292</v>
       </c>
       <c r="H26" s="31"/>
     </row>
-    <row r="27" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="27" t="s">
         <v>293</v>
       </c>
       <c r="H27" s="31"/>
     </row>
-    <row r="28" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
         <v>294</v>
       </c>
       <c r="H28" s="31"/>
     </row>
-    <row r="29" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="27" t="s">
         <v>295</v>
       </c>
       <c r="H29" s="31"/>
     </row>
-    <row r="30" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="27" t="s">
         <v>296</v>
       </c>
       <c r="H30" s="31"/>
     </row>
-    <row r="31" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="27" t="s">
         <v>297</v>
       </c>
       <c r="H31" s="31"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="18"/>
     </row>
-    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="18"/>
     </row>
-    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="18"/>
     </row>
-    <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="18"/>
     </row>
-    <row r="36" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="18"/>
     </row>
-    <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="18"/>
     </row>
-    <row r="38" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="18"/>
     </row>
-    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="18"/>
     </row>
-    <row r="40" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="18"/>
     </row>
-    <row r="41" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="18"/>
     </row>
-    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="18"/>
     </row>
-    <row r="43" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="18"/>
     </row>
-    <row r="44" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="18"/>
     </row>
-    <row r="45" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="18"/>
     </row>
-    <row r="46" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="18"/>
     </row>
-    <row r="47" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="18"/>
     </row>
-    <row r="48" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="18"/>
     </row>
-    <row r="49" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="18"/>
     </row>
-    <row r="50" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="18"/>
     </row>
-    <row r="51" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="18"/>
     </row>
-    <row r="52" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="18"/>
     </row>
-    <row r="53" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="18"/>
     </row>
-    <row r="54" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="18"/>
     </row>
-    <row r="55" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="18"/>
     </row>
-    <row r="56" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="18"/>
     </row>
-    <row r="57" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="18"/>
     </row>
-    <row r="58" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="18"/>
     </row>
-    <row r="59" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="18"/>
     </row>
-    <row r="60" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="18"/>
     </row>
-    <row r="61" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="18"/>
     </row>
-    <row r="62" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="18"/>
     </row>
-    <row r="63" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="18"/>
     </row>
-    <row r="64" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="18"/>
     </row>
-    <row r="65" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="18"/>
     </row>
-    <row r="66" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="18"/>
     </row>
-    <row r="67" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="18"/>
     </row>
-    <row r="68" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="18"/>
     </row>
-    <row r="69" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="18"/>
     </row>
-    <row r="70" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="18"/>
     </row>
-    <row r="71" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="18"/>
     </row>
-    <row r="72" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="18"/>
     </row>
-    <row r="73" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="18"/>
     </row>
-    <row r="74" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="18"/>
     </row>
-    <row r="75" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="18"/>
     </row>
-    <row r="76" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="18"/>
     </row>
-    <row r="77" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="18"/>
     </row>
-    <row r="78" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="18"/>
     </row>
-    <row r="79" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="18"/>
     </row>
-    <row r="80" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="18"/>
     </row>
-    <row r="81" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="18"/>
     </row>
-    <row r="82" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="18"/>
     </row>
-    <row r="83" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="18"/>
     </row>
-    <row r="84" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="18"/>
     </row>
-    <row r="85" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="18"/>
     </row>
-    <row r="86" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="18"/>
     </row>
-    <row r="87" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="18"/>
     </row>
-    <row r="88" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="18"/>
     </row>
-    <row r="89" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="18"/>
     </row>
-    <row r="90" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="18"/>
     </row>
-    <row r="91" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="18"/>
     </row>
-    <row r="92" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="18"/>
     </row>
-    <row r="93" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="18"/>
     </row>
   </sheetData>
@@ -13049,14 +13049,14 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -13064,7 +13064,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -13072,7 +13072,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -13080,7 +13080,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -13088,7 +13088,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -13096,7 +13096,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -13104,7 +13104,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -13112,7 +13112,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -13120,12 +13120,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -13133,7 +13133,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -13141,12 +13141,12 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -13154,7 +13154,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -13162,7 +13162,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -13170,7 +13170,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4</v>
       </c>
@@ -13178,12 +13178,12 @@
         <v>266</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -13191,7 +13191,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -13199,12 +13199,12 @@
         <v>269</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -13212,7 +13212,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -13220,7 +13220,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Adds Jen wd and GBD mort data
</commit_message>
<xml_diff>
--- a/param_files/Epi_parameters_June_24_2020.xlsx
+++ b/param_files/Epi_parameters_June_24_2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/GitHub/epi_model_HIV_TB/param_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jross\repos\epi_model_HIV_TB\param_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274B8C43-C6CB-F948-9BDF-F1F135E1FF6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD045E84-B234-4C48-9DBD-811EC3790330}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43545" yWindow="285" windowWidth="24405" windowHeight="18675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Matched_Parameters" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,19 @@
     <definedName name="R_SET">'Set Ref'!$A$11:$B$13</definedName>
     <definedName name="TB_SET">'Set Ref'!$A$1:$B$9</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -104,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="313">
   <si>
     <t>Epidemiological data point (description)</t>
   </si>
@@ -958,55 +967,91 @@
     <t>Percentage of pop LTBI</t>
   </si>
   <si>
-    <t>Excess mortality rate HIV+ CD4 &lt;200 (No active TB) - Male</t>
-  </si>
-  <si>
-    <t>Excess mortality rate HIV+ CD4 &lt;200 (No active TB) - Female</t>
-  </si>
-  <si>
-    <t>Excess mortality HIV+ CD4 &gt;200 (No active TB) - Male</t>
-  </si>
-  <si>
-    <t>Excess mortality HIV+ CD4 &gt;200 (No active TB) - Female</t>
-  </si>
-  <si>
-    <t>Excess mortality HIV+ on ART (No active TB) - Male</t>
-  </si>
-  <si>
-    <t>Excess mortality HIV+ on ART (No active TB) - Female</t>
-  </si>
-  <si>
-    <t>Excess mortality due to active TB (HIV negative) - Male</t>
-  </si>
-  <si>
-    <t>Excess mortality due to active TB (HIV negative) - Female</t>
-  </si>
-  <si>
-    <t>Excess mortality due to active TB (HIV + CD4 &lt;200) - Male</t>
-  </si>
-  <si>
-    <t>Excess mortality due to active TB (HIV + CD4 &lt;200) - Female</t>
-  </si>
-  <si>
-    <t>Excess mortality due to active TB (HIV + CD4 &gt;200) - Male</t>
-  </si>
-  <si>
-    <t>Excess mortality due to active TB (HIV + CD4 &gt;200) - Female</t>
-  </si>
-  <si>
-    <t>Excess mortality due to active TB (HIV + on ART) - Male</t>
-  </si>
-  <si>
-    <t>Excess mortality due to active TB (HIV + on ART) - Female</t>
-  </si>
-  <si>
-    <t>Background mortality rate (HIV negative and no active TB)-Male</t>
-  </si>
-  <si>
-    <t>Background mortality rate (HIV negative and no active TB)- Female</t>
-  </si>
-  <si>
-    <t>Jen to input these as proportion of the population in the compartment</t>
+    <t>All-cause mortality rate per 100,000 ages 15-49 male</t>
+  </si>
+  <si>
+    <t>GBD 2017</t>
+  </si>
+  <si>
+    <t>cause_id 294</t>
+  </si>
+  <si>
+    <t>location_id 196 (South Africa)</t>
+  </si>
+  <si>
+    <t>All-cause mortality rate per 100,000 ages 15-49 female</t>
+  </si>
+  <si>
+    <t>HIV deaths due to causes other than TB mortality rate per 100,000 ages 15-49 male</t>
+  </si>
+  <si>
+    <t>cause_id 300</t>
+  </si>
+  <si>
+    <t>HIV deaths due to causes other than TB mortality rate per 100,000 ages 15-49 female</t>
+  </si>
+  <si>
+    <t>HIV/TB mortality rate per 100,000  for drug-susceptible TB age 15-49 male</t>
+  </si>
+  <si>
+    <t>HIV/TB mortality rate per 100,000  for drug-susceptible TB age 15-49 female</t>
+  </si>
+  <si>
+    <t>All HIV mortality rate per 100,000 ages 15-49 male</t>
+  </si>
+  <si>
+    <t>cause_id 298</t>
+  </si>
+  <si>
+    <t>cause_id 948</t>
+  </si>
+  <si>
+    <t>HIV/TB mortality rate per 100,000  for MDR TB age 15-49 male</t>
+  </si>
+  <si>
+    <t>HIV/TB mortality rate per 100,000  for MDR TB age 15-49 female</t>
+  </si>
+  <si>
+    <t>cause_id 949</t>
+  </si>
+  <si>
+    <t>HIV/TB mortality rate per 100,000  for XDR TB age 15-49 male</t>
+  </si>
+  <si>
+    <t>HIV/TB mortality rate per 100,000  for XDR TB age 15-49 female</t>
+  </si>
+  <si>
+    <t>cause_id 950</t>
+  </si>
+  <si>
+    <t>TB mortality rate per 100,000 (not HIV) age 15-49 male</t>
+  </si>
+  <si>
+    <t>Confirmed units for rates as per 100,000 population against GBD compare.</t>
+  </si>
+  <si>
+    <t>Drug-susceptible TB mortality rate per 100,000 (not HIV) age 15-49 male</t>
+  </si>
+  <si>
+    <t>MDR TB mortality rate per 100,000 (not HIV) age 15-49 male</t>
+  </si>
+  <si>
+    <t>Drug-susceptible TB mortality rate per 100,000 (not HIV) age 15-49 female</t>
+  </si>
+  <si>
+    <t>XDR TB mortality rate per 100,000 (not HIV) age 15-49 male</t>
+  </si>
+  <si>
+    <t>cause_id 297</t>
+  </si>
+  <si>
+    <t>cause_id 934</t>
+  </si>
+  <si>
+    <t>cause_id 946</t>
+  </si>
+  <si>
+    <t>cause_id 947</t>
   </si>
 </sst>
 </file>
@@ -1500,35 +1545,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="K179" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <pane xSplit="10" ySplit="1" topLeftCell="K155" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K188" sqref="K188"/>
+      <selection pane="bottomRight" activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="69.33203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="53" style="9" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="7.83203125" style="9" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="7.796875" style="9" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="9" hidden="1" customWidth="1"/>
     <col min="6" max="7" width="15" style="9" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="26" style="9" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" style="9" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="22.33203125" style="9" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="9" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" style="9" customWidth="1"/>
-    <col min="13" max="13" width="20.5" style="9" customWidth="1"/>
+    <col min="12" max="12" width="17.796875" style="9" customWidth="1"/>
+    <col min="13" max="13" width="20.46484375" style="9" customWidth="1"/>
     <col min="14" max="14" width="28.6640625" style="9" customWidth="1"/>
     <col min="15" max="15" width="29" style="10" customWidth="1"/>
-    <col min="16" max="16384" width="8.83203125" style="10"/>
+    <col min="16" max="16384" width="8.796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="7" customFormat="1" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1575,7 +1619,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A2" s="20" t="s">
         <v>15</v>
       </c>
@@ -1603,7 +1647,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A3" s="20" t="s">
         <v>19</v>
       </c>
@@ -1631,7 +1675,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A4" s="20" t="s">
         <v>20</v>
       </c>
@@ -1659,7 +1703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A5" s="20" t="s">
         <v>23</v>
       </c>
@@ -1687,7 +1731,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A6" s="20" t="s">
         <v>24</v>
       </c>
@@ -1715,7 +1759,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A7" s="20" t="s">
         <v>27</v>
       </c>
@@ -1743,7 +1787,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A8" s="20" t="s">
         <v>28</v>
       </c>
@@ -1774,7 +1818,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
         <v>32</v>
       </c>
@@ -1806,7 +1850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>33</v>
       </c>
@@ -1838,7 +1882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A11" s="20" t="s">
         <v>34</v>
       </c>
@@ -1870,7 +1914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A12" s="20" t="s">
         <v>35</v>
       </c>
@@ -1898,7 +1942,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A13" s="20" t="s">
         <v>39</v>
       </c>
@@ -1920,7 +1964,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A14" s="20" t="s">
         <v>41</v>
       </c>
@@ -1957,7 +2001,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A15" s="20" t="s">
         <v>45</v>
       </c>
@@ -1994,7 +2038,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A16" s="20" t="s">
         <v>46</v>
       </c>
@@ -2034,7 +2078,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A17" s="20" t="s">
         <v>49</v>
       </c>
@@ -2074,7 +2118,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A18" s="20" t="s">
         <v>50</v>
       </c>
@@ -2114,7 +2158,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A19" s="20" t="s">
         <v>51</v>
       </c>
@@ -2154,7 +2198,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A20" s="20" t="s">
         <v>52</v>
       </c>
@@ -2194,7 +2238,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A21" s="20" t="s">
         <v>53</v>
       </c>
@@ -2234,7 +2278,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A22" s="20" t="s">
         <v>54</v>
       </c>
@@ -2271,7 +2315,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A23" s="20" t="s">
         <v>55</v>
       </c>
@@ -2308,7 +2352,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A24" s="20" t="s">
         <v>56</v>
       </c>
@@ -2348,7 +2392,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A25" s="20" t="s">
         <v>58</v>
       </c>
@@ -2388,7 +2432,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A26" s="20" t="s">
         <v>59</v>
       </c>
@@ -2428,7 +2472,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A27" s="20" t="s">
         <v>60</v>
       </c>
@@ -2468,7 +2512,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A28" s="20" t="s">
         <v>61</v>
       </c>
@@ -2505,7 +2549,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A29" s="20" t="s">
         <v>62</v>
       </c>
@@ -2542,7 +2586,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A30" s="20" t="s">
         <v>63</v>
       </c>
@@ -2579,7 +2623,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A31" s="20" t="s">
         <v>64</v>
       </c>
@@ -2616,7 +2660,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A32" s="20" t="s">
         <v>65</v>
       </c>
@@ -2653,7 +2697,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A33" s="20" t="s">
         <v>66</v>
       </c>
@@ -2690,7 +2734,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A34" s="20" t="s">
         <v>67</v>
       </c>
@@ -2727,7 +2771,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A35" s="20" t="s">
         <v>68</v>
       </c>
@@ -2764,7 +2808,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A36" s="20" t="s">
         <v>69</v>
       </c>
@@ -2801,7 +2845,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A37" s="20" t="s">
         <v>70</v>
       </c>
@@ -2838,7 +2882,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A38" s="20" t="s">
         <v>71</v>
       </c>
@@ -2875,7 +2919,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A39" s="20" t="s">
         <v>73</v>
       </c>
@@ -2912,7 +2956,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A40" s="20" t="s">
         <v>74</v>
       </c>
@@ -2952,7 +2996,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A41" s="20" t="s">
         <v>76</v>
       </c>
@@ -2992,7 +3036,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A42" s="20" t="s">
         <v>77</v>
       </c>
@@ -3032,7 +3076,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A43" s="20" t="s">
         <v>78</v>
       </c>
@@ -3072,7 +3116,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A44" s="20" t="s">
         <v>79</v>
       </c>
@@ -3112,7 +3156,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A45" s="20" t="s">
         <v>80</v>
       </c>
@@ -3152,7 +3196,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A46" s="20" t="s">
         <v>81</v>
       </c>
@@ -3192,7 +3236,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A47" s="20" t="s">
         <v>82</v>
       </c>
@@ -3232,7 +3276,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A48" s="20" t="s">
         <v>83</v>
       </c>
@@ -3269,7 +3313,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A49" s="20" t="s">
         <v>84</v>
       </c>
@@ -3306,7 +3350,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A50" s="20" t="s">
         <v>85</v>
       </c>
@@ -3343,7 +3387,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A51" s="20" t="s">
         <v>86</v>
       </c>
@@ -3380,7 +3424,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A52" s="20" t="s">
         <v>87</v>
       </c>
@@ -3417,7 +3461,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A53" s="20" t="s">
         <v>88</v>
       </c>
@@ -3454,7 +3498,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A54" s="20" t="s">
         <v>89</v>
       </c>
@@ -3491,7 +3535,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A55" s="20" t="s">
         <v>91</v>
       </c>
@@ -3528,7 +3572,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A56" s="20" t="s">
         <v>92</v>
       </c>
@@ -3565,7 +3609,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A57" s="20" t="s">
         <v>93</v>
       </c>
@@ -3602,7 +3646,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A58" s="20" t="s">
         <v>94</v>
       </c>
@@ -3639,7 +3683,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A59" s="20" t="s">
         <v>95</v>
       </c>
@@ -3676,7 +3720,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A60" s="20" t="s">
         <v>96</v>
       </c>
@@ -3713,7 +3757,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A61" s="20" t="s">
         <v>97</v>
       </c>
@@ -3750,7 +3794,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A62" s="20" t="s">
         <v>98</v>
       </c>
@@ -3787,7 +3831,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A63" s="20" t="s">
         <v>99</v>
       </c>
@@ -3824,7 +3868,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A64" s="20" t="s">
         <v>100</v>
       </c>
@@ -3861,7 +3905,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A65" s="20" t="s">
         <v>101</v>
       </c>
@@ -3898,7 +3942,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A66" s="20" t="s">
         <v>102</v>
       </c>
@@ -3935,7 +3979,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A67" s="20" t="s">
         <v>103</v>
       </c>
@@ -3972,7 +4016,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A68" s="20" t="s">
         <v>104</v>
       </c>
@@ -4009,7 +4053,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A69" s="20" t="s">
         <v>105</v>
       </c>
@@ -4046,7 +4090,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A70" s="20" t="s">
         <v>106</v>
       </c>
@@ -4083,7 +4127,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A71" s="20" t="s">
         <v>107</v>
       </c>
@@ -4120,7 +4164,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A72" s="20" t="s">
         <v>108</v>
       </c>
@@ -4157,7 +4201,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A73" s="20" t="s">
         <v>109</v>
       </c>
@@ -4194,7 +4238,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A74" s="20" t="s">
         <v>110</v>
       </c>
@@ -4231,7 +4275,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A75" s="20" t="s">
         <v>111</v>
       </c>
@@ -4268,7 +4312,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A76" s="20" t="s">
         <v>112</v>
       </c>
@@ -4305,7 +4349,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A77" s="20" t="s">
         <v>113</v>
       </c>
@@ -4342,7 +4386,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A78" s="20" t="s">
         <v>114</v>
       </c>
@@ -4379,7 +4423,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A79" s="20" t="s">
         <v>115</v>
       </c>
@@ -4416,7 +4460,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A80" s="20" t="s">
         <v>116</v>
       </c>
@@ -4453,7 +4497,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A81" s="20" t="s">
         <v>117</v>
       </c>
@@ -4490,7 +4534,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A82" s="20" t="s">
         <v>118</v>
       </c>
@@ -4527,7 +4571,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" ht="63" x14ac:dyDescent="0.45">
       <c r="A83" s="20" t="s">
         <v>119</v>
       </c>
@@ -4564,7 +4608,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A84" s="20" t="s">
         <v>120</v>
       </c>
@@ -4601,7 +4645,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A85" s="20" t="s">
         <v>121</v>
       </c>
@@ -4638,7 +4682,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A86" s="20" t="s">
         <v>122</v>
       </c>
@@ -4663,7 +4707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A87" s="20" t="s">
         <v>122</v>
       </c>
@@ -4688,7 +4732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A88" s="20" t="s">
         <v>124</v>
       </c>
@@ -4719,7 +4763,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A89" s="20" t="s">
         <v>127</v>
       </c>
@@ -4750,7 +4794,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A90" s="20" t="s">
         <v>128</v>
       </c>
@@ -4781,7 +4825,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A91" s="20" t="s">
         <v>129</v>
       </c>
@@ -4812,7 +4856,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A92" s="20" t="s">
         <v>130</v>
       </c>
@@ -4843,7 +4887,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A93" s="20" t="s">
         <v>131</v>
       </c>
@@ -4874,7 +4918,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A94" s="20" t="s">
         <v>132</v>
       </c>
@@ -4901,7 +4945,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A95" s="20" t="s">
         <v>136</v>
       </c>
@@ -4925,7 +4969,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A96" s="20" t="s">
         <v>137</v>
       </c>
@@ -4949,7 +4993,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:15" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A97" s="20" t="s">
         <v>138</v>
       </c>
@@ -4973,7 +5017,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A98" s="20" t="s">
         <v>139</v>
       </c>
@@ -4999,7 +5043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A99" s="20" t="s">
         <v>141</v>
       </c>
@@ -5025,7 +5069,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A100" s="20" t="s">
         <v>142</v>
       </c>
@@ -5051,7 +5095,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A101" s="20" t="s">
         <v>143</v>
       </c>
@@ -5077,7 +5121,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A102" s="22" t="s">
         <v>274</v>
       </c>
@@ -5101,7 +5145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A103" s="20" t="s">
         <v>144</v>
       </c>
@@ -5133,7 +5177,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A104" s="20" t="s">
         <v>148</v>
       </c>
@@ -5165,7 +5209,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A105" s="20" t="s">
         <v>150</v>
       </c>
@@ -5198,7 +5242,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A106" s="20" t="s">
         <v>152</v>
       </c>
@@ -5231,7 +5275,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A107" s="20" t="s">
         <v>154</v>
       </c>
@@ -5263,7 +5307,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A108" s="20" t="s">
         <v>156</v>
       </c>
@@ -5292,7 +5336,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A109" s="20" t="s">
         <v>157</v>
       </c>
@@ -5322,7 +5366,7 @@
         <v>0.22000000000000003</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A110" s="20" t="s">
         <v>158</v>
       </c>
@@ -5352,7 +5396,7 @@
         <v>0.44000000000000006</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A111" s="20" t="s">
         <v>159</v>
       </c>
@@ -5381,7 +5425,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A112" s="20" t="s">
         <v>160</v>
       </c>
@@ -5410,7 +5454,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A113" s="20" t="s">
         <v>161</v>
       </c>
@@ -5439,7 +5483,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A114" s="20" t="s">
         <v>162</v>
       </c>
@@ -5468,7 +5512,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A115" s="20" t="s">
         <v>163</v>
       </c>
@@ -5499,7 +5543,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A116" s="20" t="s">
         <v>166</v>
       </c>
@@ -5530,7 +5574,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A117" s="20" t="s">
         <v>167</v>
       </c>
@@ -5562,7 +5606,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A118" s="20" t="s">
         <v>168</v>
       </c>
@@ -5594,7 +5638,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A119" s="20" t="s">
         <v>169</v>
       </c>
@@ -5626,7 +5670,7 @@
         <v>2.2050000000000004E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A120" s="20" t="s">
         <v>170</v>
       </c>
@@ -5658,7 +5702,7 @@
         <v>2.2050000000000004E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A121" s="20" t="s">
         <v>171</v>
       </c>
@@ -5690,7 +5734,7 @@
         <v>2.3152500000000006E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A122" s="20" t="s">
         <v>172</v>
       </c>
@@ -5722,7 +5766,7 @@
         <v>2.3152500000000006E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A123" s="20" t="s">
         <v>173</v>
       </c>
@@ -5754,7 +5798,7 @@
         <v>2.2000000000000002E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A124" s="20" t="s">
         <v>174</v>
       </c>
@@ -5786,7 +5830,7 @@
         <v>2.2000000000000002E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A125" s="20" t="s">
         <v>175</v>
       </c>
@@ -5818,7 +5862,7 @@
         <v>2.3100000000000002E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A126" s="20" t="s">
         <v>176</v>
       </c>
@@ -5850,7 +5894,7 @@
         <v>2.3100000000000002E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A127" s="20" t="s">
         <v>177</v>
       </c>
@@ -5882,7 +5926,7 @@
         <v>2.5410000000000005E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A128" s="20" t="s">
         <v>178</v>
       </c>
@@ -5914,7 +5958,7 @@
         <v>2.5410000000000005E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A129" s="20" t="s">
         <v>179</v>
       </c>
@@ -5946,7 +5990,7 @@
         <v>2.7951000000000007E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A130" s="20" t="s">
         <v>180</v>
       </c>
@@ -5978,7 +6022,7 @@
         <v>2.7951000000000007E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" ht="57" x14ac:dyDescent="0.45">
       <c r="A131" s="20" t="s">
         <v>181</v>
       </c>
@@ -6009,7 +6053,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" ht="57" x14ac:dyDescent="0.45">
       <c r="A132" s="20" t="s">
         <v>182</v>
       </c>
@@ -6041,7 +6085,7 @@
         <v>3.0746100000000009E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" ht="57" x14ac:dyDescent="0.45">
       <c r="A133" s="20" t="s">
         <v>183</v>
       </c>
@@ -6073,7 +6117,7 @@
         <v>2.2000000000000002E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" ht="57" x14ac:dyDescent="0.45">
       <c r="A134" s="20" t="s">
         <v>184</v>
       </c>
@@ -6105,7 +6149,7 @@
         <v>3.3820710000000011E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" ht="57" x14ac:dyDescent="0.45">
       <c r="A135" s="20" t="s">
         <v>185</v>
       </c>
@@ -6137,7 +6181,7 @@
         <v>2.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" ht="57" x14ac:dyDescent="0.45">
       <c r="A136" s="20" t="s">
         <v>186</v>
       </c>
@@ -6169,7 +6213,7 @@
         <v>3.7202781000000018E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" ht="57" x14ac:dyDescent="0.45">
       <c r="A137" s="20" t="s">
         <v>187</v>
       </c>
@@ -6201,7 +6245,7 @@
         <v>2.6620000000000005E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" ht="57" x14ac:dyDescent="0.45">
       <c r="A138" s="20" t="s">
         <v>188</v>
       </c>
@@ -6233,7 +6277,7 @@
         <v>4.092305910000002E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A139" s="20" t="s">
         <v>189</v>
       </c>
@@ -6265,7 +6309,7 @@
         <v>2.9282000000000006E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A140" s="20" t="s">
         <v>190</v>
       </c>
@@ -6297,7 +6341,7 @@
         <v>4.5015365010000023E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A141" s="20" t="s">
         <v>191</v>
       </c>
@@ -6329,7 +6373,7 @@
         <v>3.2210200000000008E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A142" s="20" t="s">
         <v>192</v>
       </c>
@@ -6361,7 +6405,7 @@
         <v>4.9516901511000029E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A143" s="20" t="s">
         <v>193</v>
       </c>
@@ -6393,7 +6437,7 @@
         <v>3.5431220000000013E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A144" s="20" t="s">
         <v>194</v>
       </c>
@@ -6425,7 +6469,7 @@
         <v>5.4468591662100038E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A145" s="20" t="s">
         <v>195</v>
       </c>
@@ -6457,7 +6501,7 @@
         <v>3.8974342000000016E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A146" s="20" t="s">
         <v>196</v>
       </c>
@@ -6489,7 +6533,7 @@
         <v>5.9915450828310048E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A147" s="20" t="s">
         <v>197</v>
       </c>
@@ -6521,7 +6565,7 @@
         <v>4.092305910000002E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A148" s="20" t="s">
         <v>198</v>
       </c>
@@ -6553,7 +6597,7 @@
         <v>6.2911223369725558E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A149" s="20" t="s">
         <v>199</v>
       </c>
@@ -6585,7 +6629,7 @@
         <v>4.2969212055000025E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A150" s="20" t="s">
         <v>200</v>
       </c>
@@ -6617,7 +6661,7 @@
         <v>6.9202345706698115E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A151" s="20" t="s">
         <v>201</v>
       </c>
@@ -6649,7 +6693,7 @@
         <v>4.7266133260500033E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A152" s="20" t="s">
         <v>202</v>
       </c>
@@ -6681,7 +6725,7 @@
         <v>7.6122580277367929E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A153" s="20" t="s">
         <v>203</v>
       </c>
@@ -6713,7 +6757,7 @@
         <v>5.1992746586550044E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A154" s="20" t="s">
         <v>204</v>
       </c>
@@ -6745,7 +6789,7 @@
         <v>8.3734838305104725E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A155" s="20" t="s">
         <v>205</v>
       </c>
@@ -6777,7 +6821,7 @@
         <v>6.7590570562515065E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A156" s="20" t="s">
         <v>206</v>
       </c>
@@ -6809,7 +6853,7 @@
         <v>0.10885528979663614</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A157" s="20" t="s">
         <v>207</v>
       </c>
@@ -6841,7 +6885,7 @@
         <v>8.7867741731269586E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A158" s="20" t="s">
         <v>208</v>
       </c>
@@ -6873,7 +6917,7 @@
         <v>0.14151187673562698</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A159" s="20" t="s">
         <v>209</v>
       </c>
@@ -6905,7 +6949,7 @@
         <v>0.11422806425065046</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A160" s="20" t="s">
         <v>210</v>
       </c>
@@ -6937,7 +6981,7 @@
         <v>0.18396543975631507</v>
       </c>
     </row>
-    <row r="161" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A161" s="20" t="s">
         <v>211</v>
       </c>
@@ -6969,7 +7013,7 @@
         <v>0.1484964835258456</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A162" s="20" t="s">
         <v>212</v>
       </c>
@@ -7001,7 +7045,7 @@
         <v>0.2391550716832096</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A163" s="20" t="s">
         <v>213</v>
       </c>
@@ -7033,7 +7077,7 @@
         <v>0.11879718682067648</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A164" s="20" t="s">
         <v>214</v>
       </c>
@@ -7065,7 +7109,7 @@
         <v>0.19132405734656768</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A165" s="20" t="s">
         <v>215</v>
       </c>
@@ -7097,7 +7141,7 @@
         <v>9.5037749456541198E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A166" s="20" t="s">
         <v>216</v>
       </c>
@@ -7129,7 +7173,7 @@
         <v>0.15305924587725417</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A167" s="20" t="s">
         <v>217</v>
       </c>
@@ -7161,7 +7205,7 @@
         <v>7.6030199565232964E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A168" s="20" t="s">
         <v>218</v>
       </c>
@@ -7193,7 +7237,7 @@
         <v>0.12244739670180334</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A169" s="20" t="s">
         <v>219</v>
       </c>
@@ -7225,7 +7269,7 @@
         <v>6.0824159652186377E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A170" s="20" t="s">
         <v>220</v>
       </c>
@@ -7257,7 +7301,7 @@
         <v>9.7957917361442673E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A171" s="20" t="s">
         <v>221</v>
       </c>
@@ -7289,7 +7333,7 @@
         <v>4.2576911756530458E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A172" s="20" t="s">
         <v>222</v>
       </c>
@@ -7321,7 +7365,7 @@
         <v>6.8570542153009867E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A173" s="20" t="s">
         <v>223</v>
       </c>
@@ -7353,7 +7397,7 @@
         <v>2.9803838229571319E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A174" s="20" t="s">
         <v>224</v>
       </c>
@@ -7385,7 +7429,7 @@
         <v>4.7999379507106907E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A175" s="20" t="s">
         <v>225</v>
       </c>
@@ -7417,7 +7461,7 @@
         <v>2.0862686760699922E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A176" s="20" t="s">
         <v>226</v>
       </c>
@@ -7449,7 +7493,7 @@
         <v>3.3599565654974829E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A177" s="20" t="s">
         <v>227</v>
       </c>
@@ -7481,7 +7525,7 @@
         <v>1.4603880732489943E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A178" s="20" t="s">
         <v>228</v>
       </c>
@@ -7513,7 +7557,7 @@
         <v>2.351969595848238E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A179" s="20" t="s">
         <v>229</v>
       </c>
@@ -7544,7 +7588,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A180" s="20" t="s">
         <v>229</v>
       </c>
@@ -7575,7 +7619,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A181" s="20" t="s">
         <v>229</v>
       </c>
@@ -7606,7 +7650,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A182" s="20" t="s">
         <v>229</v>
       </c>
@@ -7637,7 +7681,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A183" s="20" t="s">
         <v>231</v>
       </c>
@@ -7669,7 +7713,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="184" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A184" s="20" t="s">
         <v>231</v>
       </c>
@@ -7701,7 +7745,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="185" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A185" s="20" t="s">
         <v>231</v>
       </c>
@@ -7733,7 +7777,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="186" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A186" s="20" t="s">
         <v>231</v>
       </c>
@@ -7765,7 +7809,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="187" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A187" s="20" t="s">
         <v>232</v>
       </c>
@@ -7797,7 +7841,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A188" s="20" t="s">
         <v>232</v>
       </c>
@@ -7829,7 +7873,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="189" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A189" s="20" t="s">
         <v>232</v>
       </c>
@@ -7861,7 +7905,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="190" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A190" s="20" t="s">
         <v>232</v>
       </c>
@@ -7893,7 +7937,7 @@
         <v>4.7499999999999999E-3</v>
       </c>
     </row>
-    <row r="191" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A191" s="20" t="s">
         <v>233</v>
       </c>
@@ -7925,7 +7969,7 @@
         <v>1.9000000000000001E-4</v>
       </c>
     </row>
-    <row r="192" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A192" s="20" t="s">
         <v>233</v>
       </c>
@@ -7957,7 +8001,7 @@
         <v>9.5000000000000005E-5</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A193" s="20" t="s">
         <v>233</v>
       </c>
@@ -7989,7 +8033,7 @@
         <v>9.5000000000000005E-5</v>
       </c>
     </row>
-    <row r="194" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A194" s="20" t="s">
         <v>233</v>
       </c>
@@ -8022,14 +8066,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O194" xr:uid="{BC67A81D-7C1F-3D4A-875A-F60944DEF322}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="rho"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState ref="A2:O194">
+  <autoFilter ref="A1:O194" xr:uid="{BC67A81D-7C1F-3D4A-875A-F60944DEF322}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O194">
     <sortCondition ref="D2:D194"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8046,21 +8084,21 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="52.1640625" customWidth="1"/>
+    <col min="1" max="1" width="52.1328125" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="9" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="9" hidden="1" customWidth="1"/>
     <col min="4" max="5" width="15" style="9" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="26" style="9" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="22.33203125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="20.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.46484375" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.46484375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.796875" style="1" customWidth="1"/>
+    <col min="11" max="12" width="20.46484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="24" t="s">
         <v>276</v>
       </c>
@@ -8098,7 +8136,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="str">
         <f t="shared" ref="A2:A33" si="0">CONCATENATE("Population in TB compartment ",VLOOKUP(C2,TB_SET,2), " with ", VLOOKUP(D2,R_SET,2), " in HIV compartment ", VLOOKUP(E2,HIV_SET,2), " and ", VLOOKUP(F2, G_SET,2))</f>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8130,7 +8168,7 @@
         <v>32693.093583980408</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8162,7 +8200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8195,7 +8233,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8227,7 +8265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8260,7 +8298,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8293,7 +8331,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8326,7 +8364,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8359,7 +8397,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8392,7 +8430,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8425,7 +8463,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8458,7 +8496,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8491,7 +8529,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8524,7 +8562,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8557,7 +8595,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Male</v>
@@ -8590,7 +8628,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -8623,7 +8661,7 @@
         <v>1348.5901103391921</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8656,7 +8694,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -8688,7 +8726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8721,7 +8759,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -8753,7 +8791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8786,7 +8824,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8819,7 +8857,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8852,7 +8890,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8885,7 +8923,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8918,7 +8956,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8951,7 +8989,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -8984,7 +9022,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -9017,7 +9055,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -9050,7 +9088,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -9083,7 +9121,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -9116,7 +9154,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -9149,7 +9187,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="str">
         <f t="shared" ref="A34:A65" si="2">CONCATENATE("Population in TB compartment ",VLOOKUP(C34,TB_SET,2), " with ", VLOOKUP(D34,R_SET,2), " in HIV compartment ", VLOOKUP(E34,HIV_SET,2), " and ", VLOOKUP(F34, G_SET,2))</f>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9182,7 +9220,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -9214,7 +9252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9247,7 +9285,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -9279,7 +9317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9312,7 +9350,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9345,7 +9383,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9378,7 +9416,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9411,7 +9449,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9444,7 +9482,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9477,7 +9515,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9510,7 +9548,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9543,7 +9581,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9576,7 +9614,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9609,7 +9647,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9642,7 +9680,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -9675,7 +9713,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9708,7 +9746,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -9740,7 +9778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9773,7 +9811,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Uninfected, not on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -9805,7 +9843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9838,7 +9876,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9871,7 +9909,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9904,7 +9942,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9937,7 +9975,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -9970,7 +10008,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10003,7 +10041,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10036,7 +10074,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10069,7 +10107,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10102,7 +10140,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10135,7 +10173,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10168,7 +10206,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10201,7 +10239,7 @@
         <v>449.53003677973061</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="str">
         <f t="shared" ref="A66:A97" si="4">CONCATENATE("Population in TB compartment ",VLOOKUP(C66,TB_SET,2), " with ", VLOOKUP(D66,R_SET,2), " in HIV compartment ", VLOOKUP(E66,HIV_SET,2), " and ", VLOOKUP(F66, G_SET,2))</f>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10234,7 +10272,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Male</v>
@@ -10266,7 +10304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10299,7 +10337,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Male</v>
@@ -10331,7 +10369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10364,7 +10402,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10397,7 +10435,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10430,7 +10468,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10463,7 +10501,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10496,7 +10534,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10529,7 +10567,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10562,7 +10600,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10595,7 +10633,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10628,7 +10666,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10661,7 +10699,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  HIV-negative and Female</v>
@@ -10694,7 +10732,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -10727,7 +10765,7 @@
         <v>1103.391908459339</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10760,7 +10798,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Male</v>
@@ -10792,7 +10830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10825,7 +10863,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Male</v>
@@ -10857,7 +10895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10890,7 +10928,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10923,7 +10961,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10956,7 +10994,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -10989,7 +11027,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11022,7 +11060,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11055,7 +11093,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11088,7 +11126,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11121,7 +11159,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11154,7 +11192,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11187,7 +11225,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11220,7 +11258,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="str">
         <f t="shared" si="4"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11253,7 +11291,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="str">
         <f t="shared" ref="A98:A129" si="6">CONCATENATE("Population in TB compartment ",VLOOKUP(C98,TB_SET,2), " with ", VLOOKUP(D98,R_SET,2), " in HIV compartment ", VLOOKUP(E98,HIV_SET,2), " and ", VLOOKUP(F98, G_SET,2))</f>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11286,7 +11324,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A99" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  HIV-negative and Female</v>
@@ -11318,7 +11356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11351,7 +11389,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4&gt;200 and Female</v>
@@ -11383,7 +11421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11416,7 +11454,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11449,7 +11487,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11482,7 +11520,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11515,7 +11553,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11548,7 +11586,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11581,7 +11619,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A108" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11614,7 +11652,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A109" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11647,7 +11685,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A110" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11680,7 +11718,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A111" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11713,7 +11751,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A112" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11746,7 +11784,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A113" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11779,7 +11817,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A114" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, not on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11812,7 +11850,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV not on ART, CD4≤200 and Female</v>
@@ -11844,7 +11882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A116" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11877,7 +11915,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A117" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Uninfected, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11909,7 +11947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A118" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11942,7 +11980,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A119" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected recently (at risk for rapid progression) with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -11975,7 +12013,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A120" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected remotely with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12008,7 +12046,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A121" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, infected remotely with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12041,7 +12079,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A122" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, on IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12074,7 +12112,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A123" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, on IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12107,7 +12145,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A124" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Active with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12140,7 +12178,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A125" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Active with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12173,7 +12211,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A126" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Recovered/Treated with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12206,7 +12244,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A127" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  Recovered/Treated with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12239,7 +12277,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A128" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, after IPT with Drug-susceptible (DS) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12272,7 +12310,7 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A129" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Population in TB compartment  LTBI, after IPT with  Multidrug-resistant (MDR-TB) in HIV compartment  PLHIV and on ART and Female</v>
@@ -12305,264 +12343,264 @@
         <v>367.79730281977959</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B144" s="8"/>
       <c r="C144" s="8"/>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B145" s="8"/>
       <c r="C145" s="8"/>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B148" s="8"/>
       <c r="C148" s="8"/>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B149" s="8"/>
       <c r="C149" s="8"/>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B161" s="8"/>
       <c r="C161" s="8"/>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B163" s="8"/>
       <c r="C163" s="8"/>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B164" s="8"/>
       <c r="C164" s="8"/>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B165" s="8"/>
       <c r="C165" s="8"/>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B166" s="8"/>
       <c r="C166" s="8"/>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B167" s="8"/>
       <c r="C167" s="8"/>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B169" s="8"/>
       <c r="C169" s="8"/>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B171" s="8"/>
       <c r="C171" s="8"/>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B172" s="8"/>
       <c r="C172" s="8"/>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B173" s="8"/>
       <c r="C173" s="8"/>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B174" s="8"/>
       <c r="C174" s="8"/>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B175" s="8"/>
       <c r="C175" s="8"/>
     </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
     </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B179" s="8"/>
       <c r="C179" s="8"/>
     </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B180" s="8"/>
       <c r="C180" s="8"/>
     </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B181" s="8"/>
       <c r="C181" s="8"/>
     </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B182" s="8"/>
       <c r="C182" s="8"/>
     </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B183" s="8"/>
       <c r="C183" s="8"/>
     </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B184" s="8"/>
       <c r="C184" s="8"/>
     </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B185" s="8"/>
       <c r="C185" s="8"/>
     </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B187" s="8"/>
       <c r="C187" s="8"/>
     </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B188" s="8"/>
       <c r="C188" s="8"/>
     </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B189" s="8"/>
       <c r="C189" s="8"/>
     </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B190" s="8"/>
       <c r="C190" s="8"/>
     </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B191" s="8"/>
       <c r="C191" s="8"/>
     </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B192" s="8"/>
       <c r="C192" s="8"/>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B193" s="8"/>
       <c r="C193" s="8"/>
     </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B194" s="8"/>
       <c r="C194" s="8"/>
     </row>
   </sheetData>
-  <sortState ref="A2:L129">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L129">
     <sortCondition ref="F2:F129"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12571,28 +12609,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD4AF83-5BDA-B246-9A8F-C4F47C31E1D4}">
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B108352" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C111481" sqref="C111481"/>
+      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="20.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.5" customWidth="1"/>
-    <col min="8" max="8" width="15.5" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="4"/>
+    <col min="3" max="3" width="17.46484375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.796875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="20.46484375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.46484375" customWidth="1"/>
+    <col min="8" max="8" width="15.46484375" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="8.796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -12618,7 +12656,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A2" s="18" t="s">
         <v>237</v>
       </c>
@@ -12629,7 +12667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A3" s="18" t="s">
         <v>239</v>
       </c>
@@ -12640,7 +12678,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A4" s="18" t="s">
         <v>241</v>
       </c>
@@ -12651,7 +12689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="18" t="s">
         <v>243</v>
       </c>
@@ -12662,7 +12700,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="18" t="s">
         <v>243</v>
       </c>
@@ -12673,7 +12711,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="18" t="s">
         <v>243</v>
       </c>
@@ -12684,7 +12722,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="18" t="s">
         <v>243</v>
       </c>
@@ -12695,7 +12733,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A9" s="18" t="s">
         <v>248</v>
       </c>
@@ -12706,7 +12744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A10" s="25" t="s">
         <v>277</v>
       </c>
@@ -12714,7 +12752,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A11" s="25" t="s">
         <v>278</v>
       </c>
@@ -12722,7 +12760,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A12" s="25" t="s">
         <v>279</v>
       </c>
@@ -12730,7 +12768,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A13" s="25" t="s">
         <v>280</v>
       </c>
@@ -12738,7 +12776,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A14" s="27" t="s">
         <v>282</v>
       </c>
@@ -12746,294 +12784,533 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A15" s="27" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A16" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="C16">
+        <v>667.69125159867303</v>
+      </c>
+      <c r="D16">
+        <v>621.91596160486597</v>
+      </c>
+      <c r="E16">
+        <v>725.80082818748997</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G16" t="s">
+        <v>287</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A17" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="C17">
+        <v>487.71837360315601</v>
+      </c>
+      <c r="D17">
+        <v>436.91669589439499</v>
+      </c>
+      <c r="E17">
+        <v>556.03760119042602</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G17" t="s">
+        <v>287</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A18" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="C18">
+        <v>353.97451428615199</v>
+      </c>
+      <c r="D18">
+        <v>298.14022379823899</v>
+      </c>
+      <c r="E18">
+        <v>421.02666012590601</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G18" t="s">
+        <v>287</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A19" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="C19">
+        <v>328.28962708281801</v>
+      </c>
+      <c r="D19">
+        <v>275.75168655442201</v>
+      </c>
+      <c r="E19">
+        <v>397.64813504226203</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G19" t="s">
+        <v>287</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A20" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="C20">
+        <v>270.29685912212301</v>
+      </c>
+      <c r="D20">
+        <v>206.97423329835701</v>
+      </c>
+      <c r="E20">
+        <v>343.91638639716899</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G20" t="s">
+        <v>287</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A21" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C21">
+        <v>264.93621874887299</v>
+      </c>
+      <c r="D21">
+        <v>205.62683179700201</v>
+      </c>
+      <c r="E21">
+        <v>339.17910941088098</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G21" t="s">
+        <v>287</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A22" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="C22">
+        <v>76.970274789631006</v>
+      </c>
+      <c r="D22">
+        <v>48.421027847361103</v>
+      </c>
+      <c r="E22">
+        <v>109.456440346139</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G22" t="s">
+        <v>287</v>
+      </c>
+      <c r="H22" s="31" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A23" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C23">
+        <v>58.460988902228898</v>
+      </c>
+      <c r="D23">
+        <v>34.611741515461397</v>
+      </c>
+      <c r="E23">
+        <v>87.602923512240494</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G23" t="s">
+        <v>287</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A24" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="C24">
+        <v>6.5950565310523803</v>
+      </c>
+      <c r="D24">
+        <v>2.67155063488859</v>
+      </c>
+      <c r="E24">
+        <v>13.136486160221301</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G24" t="s">
+        <v>287</v>
+      </c>
+      <c r="H24" s="31" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A25" s="27" t="s">
         <v>298</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="C25">
+        <v>4.8104961798478998</v>
+      </c>
+      <c r="D25">
+        <v>1.8525923964359301</v>
+      </c>
+      <c r="E25">
+        <v>10.096949019498</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G25" t="s">
+        <v>287</v>
+      </c>
+      <c r="H25" s="31" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A26" s="27" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
-        <v>299</v>
-      </c>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
-        <v>284</v>
-      </c>
-      <c r="H18" s="31"/>
-    </row>
-    <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="C26">
+        <v>0.112323843345287</v>
+      </c>
+      <c r="D26">
+        <v>4.5985772535474097E-2</v>
+      </c>
+      <c r="E26">
+        <v>0.22960163575013601</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="H19" s="31"/>
-    </row>
-    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
-        <v>286</v>
-      </c>
-      <c r="H20" s="31"/>
-    </row>
-    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="s">
+      <c r="G26" t="s">
         <v>287</v>
       </c>
-      <c r="H21" s="31"/>
-    </row>
-    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
-        <v>288</v>
-      </c>
-      <c r="H22" s="31"/>
-    </row>
-    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="27" t="s">
-        <v>289</v>
-      </c>
-      <c r="H23" s="31"/>
-    </row>
-    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="H24" s="31"/>
-    </row>
-    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
-        <v>291</v>
-      </c>
-      <c r="H25" s="31"/>
-    </row>
-    <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="H26" s="31"/>
-    </row>
-    <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="H26" s="31" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A27" s="27" t="s">
-        <v>293</v>
-      </c>
-      <c r="H27" s="31"/>
-    </row>
-    <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>301</v>
+      </c>
+      <c r="C27">
+        <v>8.1923251867938002E-2</v>
+      </c>
+      <c r="D27">
+        <v>3.1924496573431098E-2</v>
+      </c>
+      <c r="E27">
+        <v>0.17543715890676301</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G27" t="s">
+        <v>287</v>
+      </c>
+      <c r="H27" s="31" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A28" s="27" t="s">
-        <v>294</v>
-      </c>
-      <c r="H28" s="31"/>
-    </row>
-    <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+      <c r="H28" s="31" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A29" s="27" t="s">
-        <v>295</v>
-      </c>
-      <c r="H29" s="31"/>
-    </row>
-    <row r="30" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+      <c r="H29" s="31" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A30" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="H30" s="31"/>
-    </row>
-    <row r="31" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>305</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A31" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="H31" s="31"/>
-    </row>
-    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
-    </row>
-    <row r="33" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
-    </row>
-    <row r="34" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-    </row>
-    <row r="35" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="18"/>
-    </row>
-    <row r="36" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+        <v>307</v>
+      </c>
+      <c r="H31" s="31" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A32" s="27" t="s">
+        <v>306</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A33" s="27" t="s">
+        <v>306</v>
+      </c>
+      <c r="H33" s="31" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A34" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="H34" s="31" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A35" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A36" s="18"/>
     </row>
-    <row r="37" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A37" s="18"/>
     </row>
-    <row r="38" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A38" s="18"/>
     </row>
-    <row r="39" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A39" s="18"/>
     </row>
-    <row r="40" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A40" s="18"/>
     </row>
-    <row r="41" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A41" s="18"/>
     </row>
-    <row r="42" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A42" s="18"/>
     </row>
-    <row r="43" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A43" s="18"/>
     </row>
-    <row r="44" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A44" s="18"/>
     </row>
-    <row r="45" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A45" s="18"/>
     </row>
-    <row r="46" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A46" s="18"/>
     </row>
-    <row r="47" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A47" s="18"/>
     </row>
-    <row r="48" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A48" s="18"/>
     </row>
-    <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A49" s="18"/>
     </row>
-    <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A50" s="18"/>
     </row>
-    <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A51" s="18"/>
     </row>
-    <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A52" s="18"/>
     </row>
-    <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A53" s="18"/>
     </row>
-    <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A54" s="18"/>
     </row>
-    <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A55" s="18"/>
     </row>
-    <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A56" s="18"/>
     </row>
-    <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A57" s="18"/>
     </row>
-    <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A58" s="18"/>
     </row>
-    <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A59" s="18"/>
     </row>
-    <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A60" s="18"/>
     </row>
-    <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A61" s="18"/>
     </row>
-    <row r="62" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A62" s="18"/>
     </row>
-    <row r="63" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A63" s="18"/>
     </row>
-    <row r="64" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A64" s="18"/>
     </row>
-    <row r="65" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A65" s="18"/>
     </row>
-    <row r="66" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A66" s="18"/>
     </row>
-    <row r="67" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A67" s="18"/>
     </row>
-    <row r="68" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A68" s="18"/>
     </row>
-    <row r="69" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A69" s="18"/>
     </row>
-    <row r="70" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A70" s="18"/>
     </row>
-    <row r="71" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A71" s="18"/>
     </row>
-    <row r="72" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A72" s="18"/>
     </row>
-    <row r="73" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A73" s="18"/>
     </row>
-    <row r="74" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A74" s="18"/>
     </row>
-    <row r="75" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A75" s="18"/>
     </row>
-    <row r="76" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A76" s="18"/>
     </row>
-    <row r="77" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A77" s="18"/>
     </row>
-    <row r="78" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A78" s="18"/>
     </row>
-    <row r="79" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A79" s="18"/>
     </row>
-    <row r="80" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A80" s="18"/>
     </row>
-    <row r="81" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A81" s="18"/>
     </row>
-    <row r="82" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A82" s="18"/>
     </row>
-    <row r="83" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A83" s="18"/>
     </row>
-    <row r="84" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A84" s="18"/>
     </row>
-    <row r="85" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A85" s="18"/>
     </row>
-    <row r="86" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A86" s="18"/>
     </row>
-    <row r="87" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A87" s="18"/>
     </row>
-    <row r="88" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A88" s="18"/>
     </row>
-    <row r="89" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A89" s="18"/>
     </row>
-    <row r="90" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A90" s="18"/>
     </row>
-    <row r="91" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A91" s="18"/>
     </row>
-    <row r="92" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A92" s="18"/>
     </row>
-    <row r="93" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A93" s="18"/>
+    </row>
+    <row r="94" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A94" s="18"/>
+    </row>
+    <row r="95" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A95" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13049,14 +13326,14 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -13064,7 +13341,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -13072,7 +13349,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -13080,7 +13357,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -13088,7 +13365,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -13096,7 +13373,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -13104,7 +13381,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -13112,7 +13389,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -13120,12 +13397,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1</v>
       </c>
@@ -13133,7 +13410,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>2</v>
       </c>
@@ -13141,12 +13418,12 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>1</v>
       </c>
@@ -13154,7 +13431,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>2</v>
       </c>
@@ -13162,7 +13439,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>3</v>
       </c>
@@ -13170,7 +13447,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>4</v>
       </c>
@@ -13178,12 +13455,12 @@
         <v>266</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>1</v>
       </c>
@@ -13191,7 +13468,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>2</v>
       </c>
@@ -13199,12 +13476,12 @@
         <v>269</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>1</v>
       </c>
@@ -13212,7 +13489,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>2</v>
       </c>
@@ -13220,7 +13497,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Epi_parameters file updated with GBD values
Includes updates to indirect model parameters sheet, but not yet to model matched parameters sheet.
</commit_message>
<xml_diff>
--- a/param_files/Epi_parameters_June_24_2020.xlsx
+++ b/param_files/Epi_parameters_June_24_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jross\repos\epi_model_HIV_TB\param_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD045E84-B234-4C48-9DBD-811EC3790330}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E09E81-CA83-44E0-BD25-66F067CE1B4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43545" yWindow="285" windowWidth="24405" windowHeight="18675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34755" yWindow="-7620" windowWidth="19755" windowHeight="19605" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Matched_Parameters" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="324">
   <si>
     <t>Epidemiological data point (description)</t>
   </si>
@@ -1052,13 +1052,46 @@
   </si>
   <si>
     <t>cause_id 947</t>
+  </si>
+  <si>
+    <t>TB mortality rate per 100,000 (not HIV) age 15-49 female</t>
+  </si>
+  <si>
+    <t>MDR TB mortality rate per 100,000 (not HIV) age 15-49 female</t>
+  </si>
+  <si>
+    <t>XDR TB mortality rate per 100,000 (not HIV) age 15-49 female</t>
+  </si>
+  <si>
+    <t>GBD 2018</t>
+  </si>
+  <si>
+    <t>GBD 2019</t>
+  </si>
+  <si>
+    <t>GBD 2020</t>
+  </si>
+  <si>
+    <t>GBD 2021</t>
+  </si>
+  <si>
+    <t>GBD 2022</t>
+  </si>
+  <si>
+    <t>GBD 2023</t>
+  </si>
+  <si>
+    <t>GBD 2024</t>
+  </si>
+  <si>
+    <t>GBD 2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1125,6 +1158,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -12612,10 +12651,10 @@
   <dimension ref="A1:I95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomRight" activeCell="G27" sqref="G27:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13072,13 +13111,43 @@
       <c r="A28" s="27" t="s">
         <v>303</v>
       </c>
+      <c r="C28">
+        <v>32.781908989999998</v>
+      </c>
+      <c r="D28">
+        <v>29.630786910000001</v>
+      </c>
+      <c r="E28">
+        <v>36.915591910000003</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G28" t="s">
+        <v>287</v>
+      </c>
       <c r="H28" s="31" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A29" s="27" t="s">
-        <v>303</v>
+        <v>313</v>
+      </c>
+      <c r="C29">
+        <v>15.92630484</v>
+      </c>
+      <c r="D29">
+        <v>13.86750552</v>
+      </c>
+      <c r="E29">
+        <v>18.053657309999998</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="G29" t="s">
+        <v>287</v>
       </c>
       <c r="H29" s="31" t="s">
         <v>309</v>
@@ -13088,6 +13157,21 @@
       <c r="A30" s="27" t="s">
         <v>305</v>
       </c>
+      <c r="C30">
+        <v>30.619318209999999</v>
+      </c>
+      <c r="D30">
+        <v>27.03644954</v>
+      </c>
+      <c r="E30">
+        <v>34.821362049999998</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G30" t="s">
+        <v>287</v>
+      </c>
       <c r="H30" s="31" t="s">
         <v>310</v>
       </c>
@@ -13096,6 +13180,21 @@
       <c r="A31" s="27" t="s">
         <v>307</v>
       </c>
+      <c r="C31">
+        <v>14.90405754</v>
+      </c>
+      <c r="D31">
+        <v>12.80162367</v>
+      </c>
+      <c r="E31">
+        <v>17.08584523</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="G31" t="s">
+        <v>287</v>
+      </c>
       <c r="H31" s="31" t="s">
         <v>310</v>
       </c>
@@ -13104,13 +13203,43 @@
       <c r="A32" s="27" t="s">
         <v>306</v>
       </c>
+      <c r="C32">
+        <v>2.1263778709999999</v>
+      </c>
+      <c r="D32">
+        <v>0.99031739500000004</v>
+      </c>
+      <c r="E32">
+        <v>3.7960577139999998</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G32" t="s">
+        <v>287</v>
+      </c>
       <c r="H32" s="31" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A33" s="27" t="s">
-        <v>306</v>
+        <v>314</v>
+      </c>
+      <c r="C33">
+        <v>1.0051327029999999</v>
+      </c>
+      <c r="D33">
+        <v>0.49495520500000001</v>
+      </c>
+      <c r="E33">
+        <v>1.8558520039999999</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="G33" t="s">
+        <v>287</v>
       </c>
       <c r="H33" s="31" t="s">
         <v>311</v>
@@ -13120,13 +13249,43 @@
       <c r="A34" s="27" t="s">
         <v>308</v>
       </c>
+      <c r="C34">
+        <v>3.6212901999999998E-2</v>
+      </c>
+      <c r="D34">
+        <v>1.7022888999999999E-2</v>
+      </c>
+      <c r="E34">
+        <v>6.5484691999999997E-2</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="G34" t="s">
+        <v>287</v>
+      </c>
       <c r="H34" s="31" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A35" s="27" t="s">
-        <v>308</v>
+        <v>315</v>
+      </c>
+      <c r="C35">
+        <v>1.7114595999999999E-2</v>
+      </c>
+      <c r="D35">
+        <v>8.2082219999999994E-3</v>
+      </c>
+      <c r="E35">
+        <v>3.1991639000000002E-2</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G35" t="s">
+        <v>287</v>
       </c>
       <c r="H35" s="31" t="s">
         <v>312</v>
@@ -13313,6 +13472,7 @@
       <c r="A95" s="18"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated mortality parameters in epi_parameters sheet
</commit_message>
<xml_diff>
--- a/param_files/Epi_parameters_June_24_2020.xlsx
+++ b/param_files/Epi_parameters_June_24_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jross\repos\epi_model_HIV_TB\param_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E09E81-CA83-44E0-BD25-66F067CE1B4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D856B17B-ADA0-4985-B798-FCE2D7CD43AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34755" yWindow="-7620" windowWidth="19755" windowHeight="19605" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36720" yWindow="-7755" windowWidth="33495" windowHeight="20295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Matched_Parameters" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="335">
   <si>
     <t>Epidemiological data point (description)</t>
   </si>
@@ -1085,6 +1085,39 @@
   </si>
   <si>
     <t>GBD 2025</t>
+  </si>
+  <si>
+    <t>Same as baseline</t>
+  </si>
+  <si>
+    <t>Handwavy 5x baseline, establishes a ref rate for PLHIV not on ART, CD4&gt;200</t>
+  </si>
+  <si>
+    <t>Handwavy 1.2x baseline, ref rate for PLHIV on ART</t>
+  </si>
+  <si>
+    <t>Handwavy 10x baseline, ref rate for CD4 &lt;=200</t>
+  </si>
+  <si>
+    <t>Same as ref rate for PLHIV, CD4 &gt;200</t>
+  </si>
+  <si>
+    <t>Same as ref rate for PLHIV, CD4≤200</t>
+  </si>
+  <si>
+    <t>Same as ref rate for PLHIV on ART</t>
+  </si>
+  <si>
+    <t>Crude calculation from GBD = baseline mortality for males (no HIV or TB)</t>
+  </si>
+  <si>
+    <t>Crude calculation from GBD = baseline mortality for females (no HIV or TB)</t>
+  </si>
+  <si>
+    <t>TB-specific baseline</t>
+  </si>
+  <si>
+    <t>Handwavy</t>
   </si>
 </sst>
 </file>
@@ -1219,7 +1252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1304,6 +1337,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1586,11 +1622,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O194"/>
   <sheetViews>
-    <sheetView zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="K155" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A133" sqref="A133"/>
+      <selection pane="bottomRight" activeCell="M177" sqref="M177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1606,7 +1642,7 @@
     <col min="11" max="11" width="20" style="9" customWidth="1"/>
     <col min="12" max="12" width="17.796875" style="9" customWidth="1"/>
     <col min="13" max="13" width="20.46484375" style="9" customWidth="1"/>
-    <col min="14" max="14" width="28.6640625" style="9" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="9" customWidth="1"/>
     <col min="15" max="15" width="29" style="10" customWidth="1"/>
     <col min="16" max="16384" width="8.796875" style="10"/>
   </cols>
@@ -5493,7 +5529,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A113" s="20" t="s">
         <v>161</v>
       </c>
@@ -5522,7 +5558,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A114" s="20" t="s">
         <v>162</v>
       </c>
@@ -5551,7 +5587,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A115" s="20" t="s">
         <v>163</v>
       </c>
@@ -5578,11 +5614,14 @@
         <f t="shared" si="7"/>
         <v>mu_1,1,1</v>
       </c>
-      <c r="K115" s="23">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K115" s="11">
+        <v>3.3E-3</v>
+      </c>
+      <c r="O115" s="10" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A116" s="20" t="s">
         <v>166</v>
       </c>
@@ -5609,11 +5648,15 @@
         <f t="shared" si="7"/>
         <v>mu_1,1,2</v>
       </c>
-      <c r="K116" s="23">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K116" s="11">
+        <f>0.0019</f>
+        <v>1.9E-3</v>
+      </c>
+      <c r="O116" s="10" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A117" s="20" t="s">
         <v>167</v>
       </c>
@@ -5640,12 +5683,15 @@
         <f t="shared" si="7"/>
         <v>mu_1,2,1</v>
       </c>
-      <c r="K117" s="23">
-        <f>K115*1.05</f>
-        <v>2.1000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K117" s="11">
+        <f>K115*5</f>
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="O117" s="10" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A118" s="20" t="s">
         <v>168</v>
       </c>
@@ -5672,12 +5718,15 @@
         <f t="shared" si="7"/>
         <v>mu_1,2,2</v>
       </c>
-      <c r="K118" s="23">
-        <f t="shared" ref="K118:K122" si="9">K116*1.05</f>
-        <v>2.1000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K118" s="11">
+        <f>K116*5</f>
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="O118" s="10" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A119" s="20" t="s">
         <v>169</v>
       </c>
@@ -5704,12 +5753,15 @@
         <f t="shared" si="7"/>
         <v>mu_1,3,1</v>
       </c>
-      <c r="K119" s="23">
-        <f t="shared" si="9"/>
-        <v>2.2050000000000004E-2</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K119" s="11">
+        <f>K115*10</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="O119" s="10" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A120" s="20" t="s">
         <v>170</v>
       </c>
@@ -5736,12 +5788,15 @@
         <f t="shared" si="7"/>
         <v>mu_1,3,2</v>
       </c>
-      <c r="K120" s="23">
-        <f t="shared" si="9"/>
-        <v>2.2050000000000004E-2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K120" s="11">
+        <f>K116*10</f>
+        <v>1.9E-2</v>
+      </c>
+      <c r="O120" s="10" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A121" s="20" t="s">
         <v>171</v>
       </c>
@@ -5768,12 +5823,15 @@
         <f t="shared" si="7"/>
         <v>mu_1,4,1</v>
       </c>
-      <c r="K121" s="23">
-        <f t="shared" si="9"/>
-        <v>2.3152500000000006E-2</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K121" s="11">
+        <f>K115*1.2</f>
+        <v>3.96E-3</v>
+      </c>
+      <c r="O121" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A122" s="20" t="s">
         <v>172</v>
       </c>
@@ -5800,12 +5858,15 @@
         <f t="shared" si="7"/>
         <v>mu_1,4,2</v>
       </c>
-      <c r="K122" s="23">
-        <f t="shared" si="9"/>
-        <v>2.3152500000000006E-2</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K122" s="11">
+        <f>K116*1.2</f>
+        <v>2.2799999999999999E-3</v>
+      </c>
+      <c r="O122" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A123" s="20" t="s">
         <v>173</v>
       </c>
@@ -5832,12 +5893,15 @@
         <f t="shared" si="7"/>
         <v>mu_2,1,1</v>
       </c>
-      <c r="K123" s="23">
-        <f>K115*1.1</f>
-        <v>2.2000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K123" s="11">
+        <f>K115</f>
+        <v>3.3E-3</v>
+      </c>
+      <c r="O123" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A124" s="20" t="s">
         <v>174</v>
       </c>
@@ -5864,12 +5928,15 @@
         <f t="shared" si="7"/>
         <v>mu_2,1,2</v>
       </c>
-      <c r="K124" s="23">
-        <f t="shared" ref="K124:K125" si="10">K116*1.1</f>
-        <v>2.2000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K124" s="11">
+        <f>K116</f>
+        <v>1.9E-3</v>
+      </c>
+      <c r="O124" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A125" s="20" t="s">
         <v>175</v>
       </c>
@@ -5896,12 +5963,15 @@
         <f t="shared" si="7"/>
         <v>mu_2,2,1</v>
       </c>
-      <c r="K125" s="23">
-        <f t="shared" si="10"/>
-        <v>2.3100000000000002E-2</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K125" s="11">
+        <f>K117</f>
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="O125" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A126" s="20" t="s">
         <v>176</v>
       </c>
@@ -5928,12 +5998,15 @@
         <f t="shared" si="7"/>
         <v>mu_2,2,2</v>
       </c>
-      <c r="K126" s="23">
-        <f>K118*1.1</f>
-        <v>2.3100000000000002E-2</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K126" s="11">
+        <f>K118</f>
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="O126" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A127" s="20" t="s">
         <v>177</v>
       </c>
@@ -5960,13 +6033,16 @@
         <f t="shared" si="7"/>
         <v>mu_2,3,1</v>
       </c>
-      <c r="K127" s="23">
-        <f t="shared" ref="K127:K154" si="11">K125*1.1</f>
-        <v>2.5410000000000005E-2</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
-      <c r="A128" s="20" t="s">
+      <c r="K127" s="11">
+        <f>K119</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="O127" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="A128" s="32" t="s">
         <v>178</v>
       </c>
       <c r="B128" s="9" t="str">
@@ -5992,12 +6068,15 @@
         <f t="shared" si="7"/>
         <v>mu_2,3,2</v>
       </c>
-      <c r="K128" s="23">
-        <f t="shared" si="11"/>
-        <v>2.5410000000000005E-2</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K128" s="11">
+        <f>K120</f>
+        <v>1.9E-2</v>
+      </c>
+      <c r="O128" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A129" s="20" t="s">
         <v>179</v>
       </c>
@@ -6024,12 +6103,15 @@
         <f t="shared" si="7"/>
         <v>mu_2,4,1</v>
       </c>
-      <c r="K129" s="23">
-        <f t="shared" si="11"/>
-        <v>2.7951000000000007E-2</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K129" s="11">
+        <f>K121</f>
+        <v>3.96E-3</v>
+      </c>
+      <c r="O129" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A130" s="20" t="s">
         <v>180</v>
       </c>
@@ -6053,15 +6135,18 @@
         <v>2</v>
       </c>
       <c r="J130" s="9" t="str">
-        <f t="shared" ref="J130:J161" si="12">CONCATENATE(C130, "_", E130, IF(E130&lt;&gt;"",",",""), F130, IF(F130&lt;&gt;"",",",""),  G130, IF(G130&lt;&gt;"",",",""),  H130, IF(I130&lt;&gt;"","(",""), I130, IF(I130&lt;&gt;"",")",""))</f>
+        <f t="shared" ref="J130:J161" si="9">CONCATENATE(C130, "_", E130, IF(E130&lt;&gt;"",",",""), F130, IF(F130&lt;&gt;"",",",""),  G130, IF(G130&lt;&gt;"",",",""),  H130, IF(I130&lt;&gt;"","(",""), I130, IF(I130&lt;&gt;"",")",""))</f>
         <v>mu_2,4,2</v>
       </c>
-      <c r="K130" s="23">
-        <f t="shared" si="11"/>
-        <v>2.7951000000000007E-2</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+      <c r="K130" s="11">
+        <f>K122</f>
+        <v>2.2799999999999999E-3</v>
+      </c>
+      <c r="O130" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A131" s="20" t="s">
         <v>181</v>
       </c>
@@ -6085,14 +6170,18 @@
         <v>1</v>
       </c>
       <c r="J131" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_3,1,1</v>
       </c>
-      <c r="K131" s="23">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+      <c r="K131" s="11">
+        <f>K115</f>
+        <v>3.3E-3</v>
+      </c>
+      <c r="O131" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A132" s="20" t="s">
         <v>182</v>
       </c>
@@ -6116,15 +6205,18 @@
         <v>2</v>
       </c>
       <c r="J132" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_3,1,2</v>
       </c>
-      <c r="K132" s="23">
-        <f t="shared" si="11"/>
-        <v>3.0746100000000009E-2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+      <c r="K132" s="11">
+        <f>K116</f>
+        <v>1.9E-3</v>
+      </c>
+      <c r="O132" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A133" s="20" t="s">
         <v>183</v>
       </c>
@@ -6148,15 +6240,18 @@
         <v>1</v>
       </c>
       <c r="J133" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_3,2,1</v>
       </c>
-      <c r="K133" s="23">
-        <f t="shared" si="11"/>
-        <v>2.2000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+      <c r="K133" s="11">
+        <f>K117</f>
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="O133" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A134" s="20" t="s">
         <v>184</v>
       </c>
@@ -6180,15 +6275,18 @@
         <v>2</v>
       </c>
       <c r="J134" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_3,2,2</v>
       </c>
-      <c r="K134" s="23">
-        <f t="shared" si="11"/>
-        <v>3.3820710000000011E-2</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+      <c r="K134" s="11">
+        <f>K118</f>
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="O134" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A135" s="20" t="s">
         <v>185</v>
       </c>
@@ -6212,15 +6310,18 @@
         <v>1</v>
       </c>
       <c r="J135" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_3,3,1</v>
       </c>
-      <c r="K135" s="23">
-        <f t="shared" si="11"/>
-        <v>2.4200000000000003E-2</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+      <c r="K135" s="11">
+        <f>K119</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="O135" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A136" s="20" t="s">
         <v>186</v>
       </c>
@@ -6244,15 +6345,18 @@
         <v>2</v>
       </c>
       <c r="J136" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_3,3,2</v>
       </c>
-      <c r="K136" s="23">
-        <f t="shared" si="11"/>
-        <v>3.7202781000000018E-2</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+      <c r="K136" s="11">
+        <f>K120</f>
+        <v>1.9E-2</v>
+      </c>
+      <c r="O136" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A137" s="20" t="s">
         <v>187</v>
       </c>
@@ -6276,15 +6380,18 @@
         <v>1</v>
       </c>
       <c r="J137" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_3,4,1</v>
       </c>
-      <c r="K137" s="23">
-        <f t="shared" si="11"/>
-        <v>2.6620000000000005E-2</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+      <c r="K137" s="11">
+        <f>K121</f>
+        <v>3.96E-3</v>
+      </c>
+      <c r="O137" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A138" s="20" t="s">
         <v>188</v>
       </c>
@@ -6308,15 +6415,18 @@
         <v>2</v>
       </c>
       <c r="J138" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_3,4,2</v>
       </c>
-      <c r="K138" s="23">
-        <f t="shared" si="11"/>
-        <v>4.092305910000002E-2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K138" s="11">
+        <f>K122</f>
+        <v>2.2799999999999999E-3</v>
+      </c>
+      <c r="O138" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A139" s="20" t="s">
         <v>189</v>
       </c>
@@ -6340,15 +6450,18 @@
         <v>1</v>
       </c>
       <c r="J139" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_4,1,1</v>
       </c>
-      <c r="K139" s="23">
-        <f t="shared" si="11"/>
-        <v>2.9282000000000006E-2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K139" s="11">
+        <f>K115</f>
+        <v>3.3E-3</v>
+      </c>
+      <c r="O139" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A140" s="20" t="s">
         <v>190</v>
       </c>
@@ -6372,15 +6485,18 @@
         <v>2</v>
       </c>
       <c r="J140" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_4,1,2</v>
       </c>
-      <c r="K140" s="23">
-        <f t="shared" si="11"/>
-        <v>4.5015365010000023E-2</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K140" s="11">
+        <f>K116</f>
+        <v>1.9E-3</v>
+      </c>
+      <c r="O140" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A141" s="20" t="s">
         <v>191</v>
       </c>
@@ -6404,15 +6520,18 @@
         <v>1</v>
       </c>
       <c r="J141" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_4,2,1</v>
       </c>
-      <c r="K141" s="23">
-        <f t="shared" si="11"/>
-        <v>3.2210200000000008E-2</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K141" s="11">
+        <f>K117</f>
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="O141" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A142" s="20" t="s">
         <v>192</v>
       </c>
@@ -6436,15 +6555,18 @@
         <v>2</v>
       </c>
       <c r="J142" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_4,2,2</v>
       </c>
-      <c r="K142" s="23">
-        <f t="shared" si="11"/>
-        <v>4.9516901511000029E-2</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K142" s="11">
+        <f>K118</f>
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="O142" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A143" s="20" t="s">
         <v>193</v>
       </c>
@@ -6468,15 +6590,18 @@
         <v>1</v>
       </c>
       <c r="J143" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_4,3,1</v>
       </c>
-      <c r="K143" s="23">
-        <f t="shared" si="11"/>
-        <v>3.5431220000000013E-2</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K143" s="11">
+        <f>K119</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="O143" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A144" s="20" t="s">
         <v>194</v>
       </c>
@@ -6500,15 +6625,18 @@
         <v>2</v>
       </c>
       <c r="J144" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_4,3,2</v>
       </c>
-      <c r="K144" s="23">
-        <f t="shared" si="11"/>
-        <v>5.4468591662100038E-2</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K144" s="11">
+        <f>K120</f>
+        <v>1.9E-2</v>
+      </c>
+      <c r="O144" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A145" s="20" t="s">
         <v>195</v>
       </c>
@@ -6532,15 +6660,18 @@
         <v>1</v>
       </c>
       <c r="J145" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_4,4,1</v>
       </c>
-      <c r="K145" s="23">
-        <f t="shared" si="11"/>
-        <v>3.8974342000000016E-2</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K145" s="11">
+        <f>K121</f>
+        <v>3.96E-3</v>
+      </c>
+      <c r="O145" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A146" s="20" t="s">
         <v>196</v>
       </c>
@@ -6564,20 +6695,23 @@
         <v>2</v>
       </c>
       <c r="J146" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_4,4,2</v>
       </c>
-      <c r="K146" s="23">
-        <f t="shared" si="11"/>
-        <v>5.9915450828310048E-2</v>
-      </c>
-    </row>
-    <row r="147" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K146" s="11">
+        <f>K122</f>
+        <v>2.2799999999999999E-3</v>
+      </c>
+      <c r="O146" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A147" s="20" t="s">
         <v>197</v>
       </c>
       <c r="B147" s="9" t="str">
-        <f t="shared" ref="B147:B178" si="13">CONCATENATE("Mortality rates from populations in TB compartment ",VLOOKUP(E147,TB_SET,2)," and HIV compartment ",VLOOKUP(G147,HIV_SET,2)," and gender compartment ",VLOOKUP(H147,G_SET,2)," per year")</f>
+        <f t="shared" ref="B147:B178" si="10">CONCATENATE("Mortality rates from populations in TB compartment ",VLOOKUP(E147,TB_SET,2)," and HIV compartment ",VLOOKUP(G147,HIV_SET,2)," and gender compartment ",VLOOKUP(H147,G_SET,2)," per year")</f>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  HIV-negative and gender compartment Male per year</v>
       </c>
       <c r="C147" s="8" t="s">
@@ -6596,20 +6730,23 @@
         <v>1</v>
       </c>
       <c r="J147" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_5,1,1</v>
       </c>
-      <c r="K147" s="23">
-        <f>K145*1.05</f>
-        <v>4.092305910000002E-2</v>
-      </c>
-    </row>
-    <row r="148" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K147" s="11">
+        <f>K115</f>
+        <v>3.3E-3</v>
+      </c>
+      <c r="O147" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A148" s="20" t="s">
         <v>198</v>
       </c>
       <c r="B148" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  HIV-negative and gender compartment Female per year</v>
       </c>
       <c r="C148" s="8" t="s">
@@ -6628,20 +6765,23 @@
         <v>2</v>
       </c>
       <c r="J148" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_5,1,2</v>
       </c>
-      <c r="K148" s="23">
-        <f>K146*1.05</f>
-        <v>6.2911223369725558E-2</v>
-      </c>
-    </row>
-    <row r="149" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K148" s="11">
+        <f>K116</f>
+        <v>1.9E-3</v>
+      </c>
+      <c r="O148" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A149" s="20" t="s">
         <v>199</v>
       </c>
       <c r="B149" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male per year</v>
       </c>
       <c r="C149" s="8" t="s">
@@ -6660,20 +6800,23 @@
         <v>1</v>
       </c>
       <c r="J149" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_5,2,1</v>
       </c>
-      <c r="K149" s="23">
-        <f>K147*1.05</f>
-        <v>4.2969212055000025E-2</v>
-      </c>
-    </row>
-    <row r="150" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K149" s="11">
+        <f>K117</f>
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="O149" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A150" s="20" t="s">
         <v>200</v>
       </c>
       <c r="B150" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female per year</v>
       </c>
       <c r="C150" s="8" t="s">
@@ -6692,20 +6835,23 @@
         <v>2</v>
       </c>
       <c r="J150" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_5,2,2</v>
       </c>
-      <c r="K150" s="23">
-        <f t="shared" si="11"/>
-        <v>6.9202345706698115E-2</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K150" s="11">
+        <f>K118</f>
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="O150" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A151" s="20" t="s">
         <v>201</v>
       </c>
       <c r="B151" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Male per year</v>
       </c>
       <c r="C151" s="8" t="s">
@@ -6724,20 +6870,23 @@
         <v>1</v>
       </c>
       <c r="J151" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_5,3,1</v>
       </c>
-      <c r="K151" s="23">
-        <f t="shared" si="11"/>
-        <v>4.7266133260500033E-2</v>
-      </c>
-    </row>
-    <row r="152" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K151" s="11">
+        <f>K119</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="O151" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A152" s="20" t="s">
         <v>202</v>
       </c>
       <c r="B152" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Female per year</v>
       </c>
       <c r="C152" s="8" t="s">
@@ -6756,20 +6905,23 @@
         <v>2</v>
       </c>
       <c r="J152" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_5,3,2</v>
       </c>
-      <c r="K152" s="23">
-        <f t="shared" si="11"/>
-        <v>7.6122580277367929E-2</v>
-      </c>
-    </row>
-    <row r="153" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K152" s="11">
+        <f>K120</f>
+        <v>1.9E-2</v>
+      </c>
+      <c r="O152" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A153" s="20" t="s">
         <v>203</v>
       </c>
       <c r="B153" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  PLHIV and on ART and gender compartment Male per year</v>
       </c>
       <c r="C153" s="8" t="s">
@@ -6788,20 +6940,23 @@
         <v>1</v>
       </c>
       <c r="J153" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_5,4,1</v>
       </c>
-      <c r="K153" s="23">
-        <f t="shared" si="11"/>
-        <v>5.1992746586550044E-2</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K153" s="11">
+        <f>K121</f>
+        <v>3.96E-3</v>
+      </c>
+      <c r="O153" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A154" s="20" t="s">
         <v>204</v>
       </c>
       <c r="B154" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, on IPT and HIV compartment  PLHIV and on ART and gender compartment Female per year</v>
       </c>
       <c r="C154" s="8" t="s">
@@ -6820,20 +6975,23 @@
         <v>2</v>
       </c>
       <c r="J154" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_5,4,2</v>
       </c>
-      <c r="K154" s="23">
-        <f t="shared" si="11"/>
-        <v>8.3734838305104725E-2</v>
-      </c>
-    </row>
-    <row r="155" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K154" s="11">
+        <f>K122</f>
+        <v>2.2799999999999999E-3</v>
+      </c>
+      <c r="O154" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A155" s="20" t="s">
         <v>205</v>
       </c>
       <c r="B155" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  HIV-negative and gender compartment Male per year</v>
       </c>
       <c r="C155" s="8" t="s">
@@ -6852,20 +7010,23 @@
         <v>1</v>
       </c>
       <c r="J155" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_6,1,1</v>
       </c>
-      <c r="K155" s="23">
-        <f>K153*1.3</f>
-        <v>6.7590570562515065E-2</v>
-      </c>
-    </row>
-    <row r="156" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K155" s="11">
+        <f>K115*20</f>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="O155" s="10" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A156" s="20" t="s">
         <v>206</v>
       </c>
       <c r="B156" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  HIV-negative and gender compartment Female per year</v>
       </c>
       <c r="C156" s="8" t="s">
@@ -6884,20 +7045,23 @@
         <v>2</v>
       </c>
       <c r="J156" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_6,1,2</v>
       </c>
-      <c r="K156" s="23">
-        <f t="shared" ref="K156:K162" si="14">K154*1.3</f>
-        <v>0.10885528979663614</v>
-      </c>
-    </row>
-    <row r="157" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K156" s="11">
+        <f>K116*20</f>
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="O156" s="10" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A157" s="20" t="s">
         <v>207</v>
       </c>
       <c r="B157" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male per year</v>
       </c>
       <c r="C157" s="8" t="s">
@@ -6916,20 +7080,23 @@
         <v>1</v>
       </c>
       <c r="J157" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_6,2,1</v>
       </c>
-      <c r="K157" s="23">
-        <f t="shared" si="14"/>
-        <v>8.7867741731269586E-2</v>
-      </c>
-    </row>
-    <row r="158" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K157" s="11">
+        <f>K115*50</f>
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="O157" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A158" s="20" t="s">
         <v>208</v>
       </c>
       <c r="B158" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female per year</v>
       </c>
       <c r="C158" s="8" t="s">
@@ -6948,20 +7115,23 @@
         <v>2</v>
       </c>
       <c r="J158" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_6,2,2</v>
       </c>
-      <c r="K158" s="23">
-        <f t="shared" si="14"/>
-        <v>0.14151187673562698</v>
-      </c>
-    </row>
-    <row r="159" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K158" s="11">
+        <f>K116*50</f>
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="O158" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A159" s="20" t="s">
         <v>209</v>
       </c>
       <c r="B159" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Male per year</v>
       </c>
       <c r="C159" s="8" t="s">
@@ -6980,20 +7150,23 @@
         <v>1</v>
       </c>
       <c r="J159" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_6,3,1</v>
       </c>
-      <c r="K159" s="23">
-        <f t="shared" si="14"/>
-        <v>0.11422806425065046</v>
-      </c>
-    </row>
-    <row r="160" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K159" s="11">
+        <f>K115*100</f>
+        <v>0.33</v>
+      </c>
+      <c r="O159" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A160" s="20" t="s">
         <v>210</v>
       </c>
       <c r="B160" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Female per year</v>
       </c>
       <c r="C160" s="8" t="s">
@@ -7012,20 +7185,23 @@
         <v>2</v>
       </c>
       <c r="J160" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_6,3,2</v>
       </c>
-      <c r="K160" s="23">
-        <f t="shared" si="14"/>
-        <v>0.18396543975631507</v>
-      </c>
-    </row>
-    <row r="161" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K160" s="11">
+        <f>K116*100</f>
+        <v>0.19</v>
+      </c>
+      <c r="O160" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A161" s="20" t="s">
         <v>211</v>
       </c>
       <c r="B161" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  PLHIV and on ART and gender compartment Male per year</v>
       </c>
       <c r="C161" s="8" t="s">
@@ -7044,20 +7220,23 @@
         <v>1</v>
       </c>
       <c r="J161" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>mu_6,4,1</v>
       </c>
-      <c r="K161" s="23">
-        <f t="shared" si="14"/>
-        <v>0.1484964835258456</v>
-      </c>
-    </row>
-    <row r="162" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K161" s="11">
+        <f>K115*30</f>
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="O161" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A162" s="20" t="s">
         <v>212</v>
       </c>
       <c r="B162" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Active and HIV compartment  PLHIV and on ART and gender compartment Female per year</v>
       </c>
       <c r="C162" s="8" t="s">
@@ -7076,20 +7255,23 @@
         <v>2</v>
       </c>
       <c r="J162" s="9" t="str">
-        <f t="shared" ref="J162:J193" si="15">CONCATENATE(C162, "_", E162, IF(E162&lt;&gt;"",",",""), F162, IF(F162&lt;&gt;"",",",""),  G162, IF(G162&lt;&gt;"",",",""),  H162, IF(I162&lt;&gt;"","(",""), I162, IF(I162&lt;&gt;"",")",""))</f>
+        <f t="shared" ref="J162:J193" si="11">CONCATENATE(C162, "_", E162, IF(E162&lt;&gt;"",",",""), F162, IF(F162&lt;&gt;"",",",""),  G162, IF(G162&lt;&gt;"",",",""),  H162, IF(I162&lt;&gt;"","(",""), I162, IF(I162&lt;&gt;"",")",""))</f>
         <v>mu_6,4,2</v>
       </c>
-      <c r="K162" s="23">
-        <f t="shared" si="14"/>
-        <v>0.2391550716832096</v>
-      </c>
-    </row>
-    <row r="163" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K162" s="11">
+        <f>K116*30</f>
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="O162" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A163" s="20" t="s">
         <v>213</v>
       </c>
       <c r="B163" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  HIV-negative and gender compartment Male per year</v>
       </c>
       <c r="C163" s="8" t="s">
@@ -7108,20 +7290,23 @@
         <v>1</v>
       </c>
       <c r="J163" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_7,1,1</v>
       </c>
-      <c r="K163" s="23">
-        <f>K161*0.8</f>
-        <v>0.11879718682067648</v>
-      </c>
-    </row>
-    <row r="164" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K163" s="11">
+        <f>K115</f>
+        <v>3.3E-3</v>
+      </c>
+      <c r="O163" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A164" s="20" t="s">
         <v>214</v>
       </c>
       <c r="B164" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  HIV-negative and gender compartment Female per year</v>
       </c>
       <c r="C164" s="8" t="s">
@@ -7140,20 +7325,23 @@
         <v>2</v>
       </c>
       <c r="J164" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_7,1,2</v>
       </c>
-      <c r="K164" s="23">
-        <f t="shared" ref="K164:K170" si="16">K162*0.8</f>
-        <v>0.19132405734656768</v>
-      </c>
-    </row>
-    <row r="165" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K164" s="11">
+        <f>K116</f>
+        <v>1.9E-3</v>
+      </c>
+      <c r="O164" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A165" s="20" t="s">
         <v>215</v>
       </c>
       <c r="B165" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male per year</v>
       </c>
       <c r="C165" s="8" t="s">
@@ -7172,20 +7360,23 @@
         <v>1</v>
       </c>
       <c r="J165" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_7,2,1</v>
       </c>
-      <c r="K165" s="23">
-        <f t="shared" si="16"/>
-        <v>9.5037749456541198E-2</v>
-      </c>
-    </row>
-    <row r="166" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K165" s="11">
+        <f>K117</f>
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="O165" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A166" s="20" t="s">
         <v>216</v>
       </c>
       <c r="B166" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female per year</v>
       </c>
       <c r="C166" s="8" t="s">
@@ -7204,20 +7395,23 @@
         <v>2</v>
       </c>
       <c r="J166" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_7,2,2</v>
       </c>
-      <c r="K166" s="23">
-        <f t="shared" si="16"/>
-        <v>0.15305924587725417</v>
-      </c>
-    </row>
-    <row r="167" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K166" s="11">
+        <f>K118</f>
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="O166" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A167" s="20" t="s">
         <v>217</v>
       </c>
       <c r="B167" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Male per year</v>
       </c>
       <c r="C167" s="8" t="s">
@@ -7236,20 +7430,23 @@
         <v>1</v>
       </c>
       <c r="J167" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_7,3,1</v>
       </c>
-      <c r="K167" s="23">
-        <f t="shared" si="16"/>
-        <v>7.6030199565232964E-2</v>
-      </c>
-    </row>
-    <row r="168" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K167" s="11">
+        <f>K119</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="O167" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A168" s="20" t="s">
         <v>218</v>
       </c>
       <c r="B168" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Female per year</v>
       </c>
       <c r="C168" s="8" t="s">
@@ -7268,20 +7465,23 @@
         <v>2</v>
       </c>
       <c r="J168" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_7,3,2</v>
       </c>
-      <c r="K168" s="23">
-        <f t="shared" si="16"/>
-        <v>0.12244739670180334</v>
-      </c>
-    </row>
-    <row r="169" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K168" s="11">
+        <f>K120</f>
+        <v>1.9E-2</v>
+      </c>
+      <c r="O168" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A169" s="20" t="s">
         <v>219</v>
       </c>
       <c r="B169" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  PLHIV and on ART and gender compartment Male per year</v>
       </c>
       <c r="C169" s="8" t="s">
@@ -7300,20 +7500,23 @@
         <v>1</v>
       </c>
       <c r="J169" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_7,4,1</v>
       </c>
-      <c r="K169" s="23">
-        <f t="shared" si="16"/>
-        <v>6.0824159652186377E-2</v>
-      </c>
-    </row>
-    <row r="170" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K169" s="11">
+        <f>K121</f>
+        <v>3.96E-3</v>
+      </c>
+      <c r="O169" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A170" s="20" t="s">
         <v>220</v>
       </c>
       <c r="B170" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  Recovered/Treated and HIV compartment  PLHIV and on ART and gender compartment Female per year</v>
       </c>
       <c r="C170" s="8" t="s">
@@ -7332,20 +7535,23 @@
         <v>2</v>
       </c>
       <c r="J170" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_7,4,2</v>
       </c>
-      <c r="K170" s="23">
-        <f t="shared" si="16"/>
-        <v>9.7957917361442673E-2</v>
-      </c>
-    </row>
-    <row r="171" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K170" s="11">
+        <f>K122</f>
+        <v>2.2799999999999999E-3</v>
+      </c>
+      <c r="O170" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A171" s="20" t="s">
         <v>221</v>
       </c>
       <c r="B171" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  HIV-negative and gender compartment Male per year</v>
       </c>
       <c r="C171" s="8" t="s">
@@ -7364,20 +7570,23 @@
         <v>1</v>
       </c>
       <c r="J171" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_8,1,1</v>
       </c>
-      <c r="K171" s="23">
-        <f>K169*0.7</f>
-        <v>4.2576911756530458E-2</v>
-      </c>
-    </row>
-    <row r="172" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K171" s="11">
+        <f>K115</f>
+        <v>3.3E-3</v>
+      </c>
+      <c r="O171" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A172" s="20" t="s">
         <v>222</v>
       </c>
       <c r="B172" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  HIV-negative and gender compartment Female per year</v>
       </c>
       <c r="C172" s="8" t="s">
@@ -7396,20 +7605,23 @@
         <v>2</v>
       </c>
       <c r="J172" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_8,1,2</v>
       </c>
-      <c r="K172" s="23">
-        <f t="shared" ref="K172:K178" si="17">K170*0.7</f>
-        <v>6.8570542153009867E-2</v>
-      </c>
-    </row>
-    <row r="173" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K172" s="11">
+        <f>K116</f>
+        <v>1.9E-3</v>
+      </c>
+      <c r="O172" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A173" s="20" t="s">
         <v>223</v>
       </c>
       <c r="B173" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male per year</v>
       </c>
       <c r="C173" s="8" t="s">
@@ -7428,20 +7640,23 @@
         <v>1</v>
       </c>
       <c r="J173" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_8,2,1</v>
       </c>
-      <c r="K173" s="23">
-        <f t="shared" si="17"/>
-        <v>2.9803838229571319E-2</v>
-      </c>
-    </row>
-    <row r="174" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K173" s="11">
+        <f>K117</f>
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="O173" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A174" s="20" t="s">
         <v>224</v>
       </c>
       <c r="B174" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female per year</v>
       </c>
       <c r="C174" s="8" t="s">
@@ -7460,20 +7675,23 @@
         <v>2</v>
       </c>
       <c r="J174" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_8,2,2</v>
       </c>
-      <c r="K174" s="23">
-        <f t="shared" si="17"/>
-        <v>4.7999379507106907E-2</v>
-      </c>
-    </row>
-    <row r="175" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K174" s="11">
+        <f>K118</f>
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="O174" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A175" s="20" t="s">
         <v>225</v>
       </c>
       <c r="B175" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Male per year</v>
       </c>
       <c r="C175" s="8" t="s">
@@ -7492,20 +7710,23 @@
         <v>1</v>
       </c>
       <c r="J175" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_8,3,1</v>
       </c>
-      <c r="K175" s="23">
-        <f t="shared" si="17"/>
-        <v>2.0862686760699922E-2</v>
-      </c>
-    </row>
-    <row r="176" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="K175" s="11">
+        <f>K119</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="O175" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A176" s="20" t="s">
         <v>226</v>
       </c>
       <c r="B176" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  PLHIV not on ART, CD4≤200 and gender compartment Female per year</v>
       </c>
       <c r="C176" s="8" t="s">
@@ -7524,20 +7745,23 @@
         <v>2</v>
       </c>
       <c r="J176" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_8,3,2</v>
       </c>
-      <c r="K176" s="23">
-        <f t="shared" si="17"/>
-        <v>3.3599565654974829E-2</v>
-      </c>
-    </row>
-    <row r="177" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K176" s="11">
+        <f>K120</f>
+        <v>1.9E-2</v>
+      </c>
+      <c r="O176" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A177" s="20" t="s">
         <v>227</v>
       </c>
       <c r="B177" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  PLHIV and on ART and gender compartment Male per year</v>
       </c>
       <c r="C177" s="8" t="s">
@@ -7556,20 +7780,23 @@
         <v>1</v>
       </c>
       <c r="J177" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_8,4,1</v>
       </c>
-      <c r="K177" s="23">
-        <f t="shared" si="17"/>
-        <v>1.4603880732489943E-2</v>
-      </c>
-    </row>
-    <row r="178" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="K177" s="11">
+        <f>K121</f>
+        <v>3.96E-3</v>
+      </c>
+      <c r="O177" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A178" s="20" t="s">
         <v>228</v>
       </c>
       <c r="B178" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>Mortality rates from populations in TB compartment  LTBI, after IPT and HIV compartment  PLHIV and on ART and gender compartment Female per year</v>
       </c>
       <c r="C178" s="8" t="s">
@@ -7588,20 +7815,23 @@
         <v>2</v>
       </c>
       <c r="J178" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>mu_8,4,2</v>
       </c>
-      <c r="K178" s="23">
-        <f t="shared" si="17"/>
-        <v>2.351969595848238E-2</v>
-      </c>
-    </row>
-    <row r="179" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="K178" s="11">
+        <f>K122</f>
+        <v>2.2799999999999999E-3</v>
+      </c>
+      <c r="O178" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A179" s="20" t="s">
         <v>229</v>
       </c>
       <c r="B179" s="9" t="str">
-        <f t="shared" ref="B179:B194" si="18">CONCATENATE("Birth rate into HIV compartment ", VLOOKUP(G179, HIV_SET, 2), " and gender compartment ", VLOOKUP(H179, G_SET, 2), ", per year")</f>
+        <f t="shared" ref="B179:B194" si="12">CONCATENATE("Birth rate into HIV compartment ", VLOOKUP(G179, HIV_SET, 2), " and gender compartment ", VLOOKUP(H179, G_SET, 2), ", per year")</f>
         <v>Birth rate into HIV compartment  HIV-negative and gender compartment Male, per year</v>
       </c>
       <c r="C179" s="8" t="s">
@@ -7620,19 +7850,19 @@
         <v>1</v>
       </c>
       <c r="J179" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_1,1,1</v>
       </c>
       <c r="K179" s="23">
         <v>0.02</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A180" s="20" t="s">
         <v>229</v>
       </c>
       <c r="B180" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  HIV-negative and gender compartment Male, per year</v>
       </c>
       <c r="C180" s="8" t="s">
@@ -7651,19 +7881,19 @@
         <v>1</v>
       </c>
       <c r="J180" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_3,1,1</v>
       </c>
       <c r="K180" s="23">
         <v>0.01</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A181" s="20" t="s">
         <v>229</v>
       </c>
       <c r="B181" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  HIV-negative and gender compartment Male, per year</v>
       </c>
       <c r="C181" s="8" t="s">
@@ -7682,19 +7912,19 @@
         <v>1</v>
       </c>
       <c r="J181" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_4,1,1</v>
       </c>
       <c r="K181" s="23">
         <v>0.01</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A182" s="20" t="s">
         <v>229</v>
       </c>
       <c r="B182" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  HIV-negative and gender compartment Male, per year</v>
       </c>
       <c r="C182" s="8" t="s">
@@ -7713,19 +7943,19 @@
         <v>1</v>
       </c>
       <c r="J182" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_6,1,1</v>
       </c>
       <c r="K182" s="23">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A183" s="20" t="s">
         <v>231</v>
       </c>
       <c r="B183" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male, per year</v>
       </c>
       <c r="C183" s="8" t="s">
@@ -7744,7 +7974,7 @@
         <v>1</v>
       </c>
       <c r="J183" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_1,2,1</v>
       </c>
       <c r="K183" s="23">
@@ -7752,12 +7982,12 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="184" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A184" s="20" t="s">
         <v>231</v>
       </c>
       <c r="B184" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male, per year</v>
       </c>
       <c r="C184" s="8" t="s">
@@ -7776,20 +8006,20 @@
         <v>1</v>
       </c>
       <c r="J184" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_3,2,1</v>
       </c>
       <c r="K184" s="23">
-        <f t="shared" ref="K184:K186" si="19">K180*0.01</f>
+        <f t="shared" ref="K184:K186" si="13">K180*0.01</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="185" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A185" s="20" t="s">
         <v>231</v>
       </c>
       <c r="B185" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male, per year</v>
       </c>
       <c r="C185" s="8" t="s">
@@ -7808,20 +8038,20 @@
         <v>1</v>
       </c>
       <c r="J185" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_4,2,1</v>
       </c>
       <c r="K185" s="23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="13"/>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="186" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A186" s="20" t="s">
         <v>231</v>
       </c>
       <c r="B186" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Male, per year</v>
       </c>
       <c r="C186" s="8" t="s">
@@ -7840,20 +8070,20 @@
         <v>1</v>
       </c>
       <c r="J186" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_6,2,1</v>
       </c>
       <c r="K186" s="23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="13"/>
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="187" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A187" s="20" t="s">
         <v>232</v>
       </c>
       <c r="B187" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  HIV-negative and gender compartment Female, per year</v>
       </c>
       <c r="C187" s="8" t="s">
@@ -7872,7 +8102,7 @@
         <v>2</v>
       </c>
       <c r="J187" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_1,1,2</v>
       </c>
       <c r="K187" s="23">
@@ -7880,12 +8110,12 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A188" s="20" t="s">
         <v>232</v>
       </c>
       <c r="B188" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  HIV-negative and gender compartment Female, per year</v>
       </c>
       <c r="C188" s="8" t="s">
@@ -7904,20 +8134,20 @@
         <v>2</v>
       </c>
       <c r="J188" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_3,1,2</v>
       </c>
       <c r="K188" s="23">
-        <f t="shared" ref="K188:K194" si="20">K180*0.95</f>
+        <f t="shared" ref="K188:K194" si="14">K180*0.95</f>
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="189" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A189" s="20" t="s">
         <v>232</v>
       </c>
       <c r="B189" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  HIV-negative and gender compartment Female, per year</v>
       </c>
       <c r="C189" s="8" t="s">
@@ -7936,20 +8166,20 @@
         <v>2</v>
       </c>
       <c r="J189" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_4,1,2</v>
       </c>
       <c r="K189" s="23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="14"/>
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="190" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A190" s="20" t="s">
         <v>232</v>
       </c>
       <c r="B190" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  HIV-negative and gender compartment Female, per year</v>
       </c>
       <c r="C190" s="8" t="s">
@@ -7968,20 +8198,20 @@
         <v>2</v>
       </c>
       <c r="J190" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_6,1,2</v>
       </c>
       <c r="K190" s="23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="14"/>
         <v>4.7499999999999999E-3</v>
       </c>
     </row>
-    <row r="191" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A191" s="20" t="s">
         <v>233</v>
       </c>
       <c r="B191" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female, per year</v>
       </c>
       <c r="C191" s="8" t="s">
@@ -8000,20 +8230,20 @@
         <v>2</v>
       </c>
       <c r="J191" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_1,2,2</v>
       </c>
       <c r="K191" s="23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="14"/>
         <v>1.9000000000000001E-4</v>
       </c>
     </row>
-    <row r="192" spans="1:11" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:15" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A192" s="20" t="s">
         <v>233</v>
       </c>
       <c r="B192" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female, per year</v>
       </c>
       <c r="C192" s="8" t="s">
@@ -8032,11 +8262,11 @@
         <v>2</v>
       </c>
       <c r="J192" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_3,2,2</v>
       </c>
       <c r="K192" s="23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="14"/>
         <v>9.5000000000000005E-5</v>
       </c>
     </row>
@@ -8045,7 +8275,7 @@
         <v>233</v>
       </c>
       <c r="B193" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female, per year</v>
       </c>
       <c r="C193" s="8" t="s">
@@ -8064,11 +8294,11 @@
         <v>2</v>
       </c>
       <c r="J193" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>rho_4,2,2</v>
       </c>
       <c r="K193" s="23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="14"/>
         <v>9.5000000000000005E-5</v>
       </c>
     </row>
@@ -8077,7 +8307,7 @@
         <v>233</v>
       </c>
       <c r="B194" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>Birth rate into HIV compartment  PLHIV not on ART, CD4&gt;200 and gender compartment Female, per year</v>
       </c>
       <c r="C194" s="8" t="s">
@@ -8096,11 +8326,11 @@
         <v>2</v>
       </c>
       <c r="J194" s="9" t="str">
-        <f t="shared" ref="J194" si="21">CONCATENATE(C194, "_", E194, IF(E194&lt;&gt;"",",",""), F194, IF(F194&lt;&gt;"",",",""),  G194, IF(G194&lt;&gt;"",",",""),  H194, IF(I194&lt;&gt;"","(",""), I194, IF(I194&lt;&gt;"",")",""))</f>
+        <f t="shared" ref="J194" si="15">CONCATENATE(C194, "_", E194, IF(E194&lt;&gt;"",",",""), F194, IF(F194&lt;&gt;"",",",""),  G194, IF(G194&lt;&gt;"",",",""),  H194, IF(I194&lt;&gt;"","(",""), I194, IF(I194&lt;&gt;"",")",""))</f>
         <v>rho_6,2,2</v>
       </c>
       <c r="K194" s="23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="14"/>
         <v>4.7500000000000003E-5</v>
       </c>
     </row>
@@ -12650,11 +12880,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD4AF83-5BDA-B246-9A8F-C4F47C31E1D4}">
   <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G27" sqref="G27:G35"/>
+      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>